<commit_message>
added gearbox ratios to the corrsponding worksheets
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ElectricMotors\Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EB52AD-897C-4B49-B3E8-BF4E959CB0C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D597F7E8-DD8C-4AC5-9A8C-6FAB86AD4844}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
+    <workbookView xWindow="885" yWindow="435" windowWidth="29700" windowHeight="20415" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Application" sheetId="1" r:id="rId1"/>
+    <sheet name="Gearbox" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>Value</t>
   </si>
@@ -284,6 +285,78 @@
   <si>
     <t>Slope angle (%)</t>
   </si>
+  <si>
+    <t>F03L1-x-19</t>
+  </si>
+  <si>
+    <t>F03T1-x-19</t>
+  </si>
+  <si>
+    <t>F06L1-x-19</t>
+  </si>
+  <si>
+    <t>F06T1-x-19</t>
+  </si>
+  <si>
+    <t>F12L1-x-19</t>
+  </si>
+  <si>
+    <t>F12T</t>
+  </si>
+  <si>
+    <t>F06V1-Z-19-SX</t>
+  </si>
+  <si>
+    <t>F06V1-Z-19-HX</t>
+  </si>
+  <si>
+    <t>Max Input Speed [rpm]</t>
+  </si>
+  <si>
+    <t>Max Input Torque [Nm]</t>
+  </si>
+  <si>
+    <t>Max Output Torque [Nm]</t>
+  </si>
+  <si>
+    <t>Ratios</t>
+  </si>
+  <si>
+    <t>1.0 - 3.94</t>
+  </si>
+  <si>
+    <t>600x2</t>
+  </si>
+  <si>
+    <t>3600x2</t>
+  </si>
+  <si>
+    <t>Ve002</t>
+  </si>
+  <si>
+    <t>PS Gearbox</t>
+  </si>
+  <si>
+    <t>Planetory Gearbox</t>
+  </si>
+  <si>
+    <t>Cont. Torque [Nm]</t>
+  </si>
+  <si>
+    <t>Ve005</t>
+  </si>
+  <si>
+    <t>Ve009</t>
+  </si>
+  <si>
+    <t>Ve01/01S</t>
+  </si>
+  <si>
+    <t>VE07</t>
+  </si>
+  <si>
+    <t>Gear Ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -343,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -395,11 +468,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,6 +577,41 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,6 +619,42 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,7 +834,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$22:$E$31</c:f>
+              <c:f>Application!$E$22:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -656,7 +873,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$22:$H$31</c:f>
+              <c:f>Application!$H$22:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -768,7 +985,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$44</c:f>
+              <c:f>Application!$E$35:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -807,7 +1024,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$35:$H$44</c:f>
+              <c:f>Application!$H$35:$H$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -919,7 +1136,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$48:$E$60</c:f>
+              <c:f>Application!$E$48:$E$60</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -967,7 +1184,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$48:$H$60</c:f>
+              <c:f>Application!$H$48:$H$60</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1086,7 +1303,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1137,7 +1354,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1616,7 +1833,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$63</c:f>
+              <c:f>Application!$F$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1687,7 +1904,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$64:$E$79</c:f>
+              <c:f>Application!$E$64:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1744,7 +1961,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$64:$F$79</c:f>
+              <c:f>Application!$F$64:$F$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1811,7 +2028,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$63</c:f>
+              <c:f>Application!$G$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1882,7 +2099,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$64:$E$79</c:f>
+              <c:f>Application!$E$64:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1939,7 +2156,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$64:$G$79</c:f>
+              <c:f>Application!$G$64:$G$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2006,7 +2223,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$63</c:f>
+              <c:f>Application!$H$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2077,7 +2294,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$64:$E$79</c:f>
+              <c:f>Application!$E$64:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2134,7 +2351,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$64:$H$79</c:f>
+              <c:f>Application!$H$64:$H$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2201,7 +2418,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$63</c:f>
+              <c:f>Application!$I$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2272,7 +2489,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$64:$E$79</c:f>
+              <c:f>Application!$E$64:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2329,7 +2546,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$64:$I$79</c:f>
+              <c:f>Application!$I$64:$I$79</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2457,7 +2674,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2508,7 +2725,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2985,7 +3202,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$82</c:f>
+              <c:f>Application!$F$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3056,7 +3273,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$83:$E$108</c:f>
+              <c:f>Application!$E$83:$E$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3143,7 +3360,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$83:$F$108</c:f>
+              <c:f>Application!$F$83:$F$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3240,7 +3457,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$82</c:f>
+              <c:f>Application!$G$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3311,7 +3528,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$83:$E$108</c:f>
+              <c:f>Application!$E$83:$E$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3398,7 +3615,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$83:$G$108</c:f>
+              <c:f>Application!$G$83:$G$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3495,7 +3712,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$82</c:f>
+              <c:f>Application!$H$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3566,7 +3783,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$83:$E$108</c:f>
+              <c:f>Application!$E$83:$E$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3653,7 +3870,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$83:$H$108</c:f>
+              <c:f>Application!$H$83:$H$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3750,7 +3967,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$82</c:f>
+              <c:f>Application!$I$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3821,7 +4038,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$83:$E$108</c:f>
+              <c:f>Application!$E$83:$E$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -3908,7 +4125,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$83:$I$108</c:f>
+              <c:f>Application!$I$83:$I$108</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -4044,7 +4261,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -4095,7 +4312,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -4581,7 +4798,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$112</c:f>
+              <c:f>Application!$F$112</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4652,7 +4869,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$113:$E$128</c:f>
+              <c:f>Application!$E$113:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4709,7 +4926,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$113:$F$128</c:f>
+              <c:f>Application!$F$113:$F$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4776,7 +4993,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$112</c:f>
+              <c:f>Application!$G$112</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4847,7 +5064,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$113:$E$128</c:f>
+              <c:f>Application!$E$113:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4904,7 +5121,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$113:$G$128</c:f>
+              <c:f>Application!$G$113:$G$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4971,7 +5188,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$112</c:f>
+              <c:f>Application!$H$112</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5042,7 +5259,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$113:$E$128</c:f>
+              <c:f>Application!$E$113:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5099,7 +5316,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$113:$H$128</c:f>
+              <c:f>Application!$H$113:$H$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5166,7 +5383,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$112</c:f>
+              <c:f>Application!$I$112</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5237,7 +5454,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$113:$E$128</c:f>
+              <c:f>Application!$E$113:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5294,7 +5511,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$113:$I$128</c:f>
+              <c:f>Application!$I$113:$I$128</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5397,7 +5614,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -5448,7 +5665,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -5934,7 +6151,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$132</c:f>
+              <c:f>Application!$F$132</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6005,7 +6222,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$133:$E$148</c:f>
+              <c:f>Application!$E$133:$E$148</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6062,7 +6279,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$133:$F$148</c:f>
+              <c:f>Application!$F$133:$F$148</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6129,7 +6346,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$132</c:f>
+              <c:f>Application!$G$132</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6200,7 +6417,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$133:$E$148</c:f>
+              <c:f>Application!$E$133:$E$148</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6257,7 +6474,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$133:$G$148</c:f>
+              <c:f>Application!$G$133:$G$148</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6324,7 +6541,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$132</c:f>
+              <c:f>Application!$H$132</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6395,7 +6612,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$133:$E$148</c:f>
+              <c:f>Application!$E$133:$E$148</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6452,7 +6669,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$133:$H$148</c:f>
+              <c:f>Application!$H$133:$H$148</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6519,7 +6736,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$132</c:f>
+              <c:f>Application!$I$132</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6590,7 +6807,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$133:$E$148</c:f>
+              <c:f>Application!$E$133:$E$148</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6647,7 +6864,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$133:$I$148</c:f>
+              <c:f>Application!$I$133:$I$148</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6750,7 +6967,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -6801,7 +7018,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -7256,7 +7473,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Application!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7327,7 +7544,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$15</c:f>
+              <c:f>Application!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -7378,7 +7595,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$15</c:f>
+              <c:f>Application!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -7897,7 +8114,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$22:$E$31</c:f>
+              <c:f>Application!$E$22:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7936,7 +8153,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$F$31</c:f>
+              <c:f>Application!$F$22:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8048,7 +8265,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$44</c:f>
+              <c:f>Application!$E$35:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8087,7 +8304,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$35:$F$44</c:f>
+              <c:f>Application!$F$35:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8199,7 +8416,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$48:$E$60</c:f>
+              <c:f>Application!$E$48:$E$60</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -8247,7 +8464,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$48:$F$60</c:f>
+              <c:f>Application!$F$48:$F$60</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -8366,7 +8583,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$15</c:f>
+              <c:f>Application!$U$2:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -8417,7 +8634,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:f>Application!$T$2:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -8903,7 +9120,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$15</c:f>
+              <c:f>Application!$J$2:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -8954,7 +9171,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$15</c:f>
+              <c:f>Application!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -14177,8 +14394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335F5D5-EBE0-44CD-9439-894D8E00CE51}">
   <dimension ref="A1:U148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14200,7 +14417,7 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="27" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -14265,7 +14482,7 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="1">
         <v>0</v>
       </c>
@@ -14318,6 +14535,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="1">
+        <f>$B$15</f>
         <v>110</v>
       </c>
       <c r="T2" s="1">
@@ -14339,7 +14557,7 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="1">
         <v>2</v>
       </c>
@@ -14394,6 +14612,7 @@
         <v>21.220659078919379</v>
       </c>
       <c r="S3" s="1">
+        <f t="shared" ref="S3:S15" si="9">$B$15</f>
         <v>110</v>
       </c>
       <c r="T3" s="1">
@@ -14401,7 +14620,7 @@
         <v>6.3878356955454549</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U15" si="9">R3*S3</f>
+        <f t="shared" ref="U3:U15" si="10">R3*S3</f>
         <v>2334.2724986811318</v>
       </c>
     </row>
@@ -14415,12 +14634,12 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="1">
         <v>4</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F15" si="10">F3+$B$12*2</f>
+        <f t="shared" ref="F4:F15" si="11">F3+$B$12*2</f>
         <v>2</v>
       </c>
       <c r="G4" s="1">
@@ -14428,7 +14647,7 @@
         <v>1.78</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H15" si="11">(G4-G3)/(E4-E3)</f>
+        <f t="shared" ref="H4:H15" si="12">(G4-G3)/(E4-E3)</f>
         <v>0.39</v>
       </c>
       <c r="I4" s="1">
@@ -14470,6 +14689,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S4" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T4" s="1">
@@ -14477,7 +14697,7 @@
         <v>5.214271854229855</v>
       </c>
       <c r="U4" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14491,12 +14711,12 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="G5" s="1">
@@ -14504,11 +14724,11 @@
         <v>1.78</v>
       </c>
       <c r="H5" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I15" si="12">$I$2/G5</f>
+        <f t="shared" ref="I5:I15" si="13">$I$2/G5</f>
         <v>23019.330337078653</v>
       </c>
       <c r="J5" s="1">
@@ -14546,6 +14766,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S5" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T5" s="1">
@@ -14553,7 +14774,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14564,12 +14785,12 @@
       <c r="B6">
         <v>0.36</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="1">
         <v>8</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -14577,11 +14798,11 @@
         <v>1.78</v>
       </c>
       <c r="H6" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23019.330337078653</v>
       </c>
       <c r="J6" s="1">
@@ -14619,6 +14840,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S6" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T6" s="1">
@@ -14626,7 +14848,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14637,12 +14859,12 @@
       <c r="B7">
         <v>0.01</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G7" s="1">
@@ -14650,11 +14872,11 @@
         <v>1.78</v>
       </c>
       <c r="H7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23019.330337078653</v>
       </c>
       <c r="J7" s="1">
@@ -14692,6 +14914,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S7" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T7" s="1">
@@ -14699,7 +14922,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14710,12 +14933,12 @@
       <c r="B8">
         <v>0.4</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="1">
         <v>12</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="G8" s="1">
@@ -14723,11 +14946,11 @@
         <v>1.78</v>
       </c>
       <c r="H8" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23019.330337078653</v>
       </c>
       <c r="J8" s="1">
@@ -14765,6 +14988,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S8" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T8" s="1">
@@ -14772,7 +14996,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14786,12 +15010,12 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="1">
         <v>14</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="G9" s="1">
@@ -14799,11 +15023,11 @@
         <v>1.78</v>
       </c>
       <c r="H9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23019.330337078653</v>
       </c>
       <c r="J9" s="1">
@@ -14841,6 +15065,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S9" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T9" s="1">
@@ -14848,7 +15073,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14859,12 +15084,12 @@
       <c r="B10">
         <v>0.8</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="1">
         <v>16</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="G10" s="1">
@@ -14872,11 +15097,11 @@
         <v>1.78</v>
       </c>
       <c r="H10" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23019.330337078653</v>
       </c>
       <c r="J10" s="1">
@@ -14914,6 +15139,7 @@
         <v>37.772773160476497</v>
       </c>
       <c r="S10" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T10" s="1">
@@ -14921,7 +15147,7 @@
         <v>1.0493377633207637</v>
       </c>
       <c r="U10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4155.0050476524148</v>
       </c>
     </row>
@@ -14935,12 +15161,12 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="1">
         <v>18</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="G11" s="1">
@@ -14950,7 +15176,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>40974408</v>
       </c>
       <c r="J11" s="1">
@@ -14990,6 +15216,7 @@
         <v>2.1220659078919377E-2</v>
       </c>
       <c r="S11" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T11" s="1">
@@ -15011,30 +15238,30 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="1">
         <v>20</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="G12" s="1">
         <v>0.5</v>
       </c>
       <c r="H12" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2495</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>81948.816000000006</v>
       </c>
       <c r="J12" s="1">
         <v>5</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" ref="K12:K15" si="13">ATAN2(100, J12)</f>
+        <f t="shared" ref="K12:K15" si="14">ATAN2(100, J12)</f>
         <v>4.9958395721942765E-2</v>
       </c>
       <c r="L12" s="1">
@@ -15066,6 +15293,7 @@
         <v>10.610329539459689</v>
       </c>
       <c r="S12" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T12" s="1">
@@ -15073,7 +15301,7 @@
         <v>8.9426278344070855</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1167.1362493405659</v>
       </c>
     </row>
@@ -15087,30 +15315,30 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="1">
         <v>22</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="G13" s="1">
         <v>0.5</v>
       </c>
       <c r="H13" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>81948.816000000006</v>
       </c>
       <c r="J13" s="1">
         <v>6</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.9928155121207881E-2</v>
       </c>
       <c r="L13" s="1">
@@ -15142,6 +15370,7 @@
         <v>10.610329539459689</v>
       </c>
       <c r="S13" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T13" s="1">
@@ -15149,7 +15378,7 @@
         <v>7.3204569243368782</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1167.1362493405659</v>
       </c>
     </row>
@@ -15160,30 +15389,30 @@
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="1">
         <v>24</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="G14" s="1">
         <v>0.5</v>
       </c>
       <c r="H14" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>81948.816000000006</v>
       </c>
       <c r="J14" s="1">
         <v>7</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.9886001634642508E-2</v>
       </c>
       <c r="L14" s="1">
@@ -15215,6 +15444,7 @@
         <v>10.610329539459689</v>
       </c>
       <c r="S14" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T14" s="1">
@@ -15222,35 +15452,41 @@
         <v>8.3608041707835579</v>
       </c>
       <c r="U14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1167.1362493405659</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="14"/>
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>110</v>
+      </c>
+      <c r="D15" s="27"/>
       <c r="E15" s="1">
         <v>26</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="G15" s="1">
         <v>0.5</v>
       </c>
       <c r="H15" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>81948.816000000006</v>
       </c>
       <c r="J15" s="1">
         <v>9</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.9758174189950524E-2</v>
       </c>
       <c r="L15" s="1">
@@ -15282,6 +15518,7 @@
         <v>10.610329539459689</v>
       </c>
       <c r="S15" s="1">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="T15" s="1">
@@ -15289,44 +15526,44 @@
         <v>10.434371575380725</v>
       </c>
       <c r="U15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1167.1362493405659</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="14"/>
+      <c r="D16" s="27"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D17" s="14"/>
+      <c r="D17" s="27"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D18" s="14"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D19" s="14"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
+      <c r="D20" s="27"/>
+      <c r="E20" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
     </row>
     <row r="21" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="2" t="s">
         <v>52</v>
       </c>
@@ -15357,7 +15594,7 @@
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="8">
         <v>0</v>
       </c>
@@ -15377,7 +15614,7 @@
         <v>208</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" ref="K22:K31" si="14">H22*$J$22/$F$22</f>
+        <f t="shared" ref="K22:K31" si="15">H22*$J$22/$F$22</f>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15390,7 +15627,7 @@
         <f>B23*0.453592</f>
         <v>29483.48</v>
       </c>
-      <c r="D23" s="14"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="8">
         <v>500</v>
       </c>
@@ -15410,7 +15647,7 @@
         <v>208</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15421,7 +15658,7 @@
       <c r="C24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="14"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="8">
         <v>1000</v>
       </c>
@@ -15441,7 +15678,7 @@
         <v>208</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15453,7 +15690,7 @@
         <f>B25*0.0254</f>
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="8">
         <v>1800</v>
       </c>
@@ -15473,7 +15710,7 @@
         <v>208</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15484,7 +15721,7 @@
       <c r="C26" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="14"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="8">
         <v>2000</v>
       </c>
@@ -15501,11 +15738,11 @@
         <v>2.5130890052356021</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" ref="J26:J31" si="15">F26*$J$22/$F$22</f>
+        <f t="shared" ref="J26:J31" si="16">F26*$J$22/$F$22</f>
         <v>187.2</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15517,7 +15754,7 @@
         <f>B27*4.44822</f>
         <v>4.4482200000000001</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="8">
         <v>2500</v>
       </c>
@@ -15534,11 +15771,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J27" s="1">
+        <f t="shared" si="16"/>
+        <v>149.76</v>
+      </c>
+      <c r="K27" s="1">
         <f t="shared" si="15"/>
-        <v>149.76</v>
-      </c>
-      <c r="K27" s="1">
-        <f t="shared" si="14"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -15549,7 +15786,7 @@
       <c r="C28" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="14"/>
+      <c r="D28" s="27"/>
       <c r="E28" s="8">
         <v>3000</v>
       </c>
@@ -15566,11 +15803,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J28" s="1">
+        <f t="shared" si="16"/>
+        <v>124.8</v>
+      </c>
+      <c r="K28" s="1">
         <f t="shared" si="15"/>
-        <v>124.8</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" si="14"/>
         <v>59.428571428571445</v>
       </c>
     </row>
@@ -15582,7 +15819,7 @@
         <f>B29*2.23694</f>
         <v>23.264176000000003</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="8">
         <v>3500</v>
       </c>
@@ -15599,11 +15836,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J29" s="1">
+        <f t="shared" si="16"/>
+        <v>106.97142857142858</v>
+      </c>
+      <c r="K29" s="1">
         <f t="shared" si="15"/>
-        <v>106.97142857142858</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" si="14"/>
         <v>50.938775510204088</v>
       </c>
     </row>
@@ -15614,7 +15851,7 @@
       <c r="C30" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="14"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="8">
         <v>4000</v>
       </c>
@@ -15631,11 +15868,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J30" s="1">
+        <f t="shared" si="16"/>
+        <v>93.6</v>
+      </c>
+      <c r="K30" s="1">
         <f t="shared" si="15"/>
-        <v>93.6</v>
-      </c>
-      <c r="K30" s="1">
-        <f t="shared" si="14"/>
         <v>44.571428571428577</v>
       </c>
     </row>
@@ -15647,7 +15884,7 @@
         <f>B31*0.277778</f>
         <v>1.7777792000000003</v>
       </c>
-      <c r="D31" s="14"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="8">
         <v>4500</v>
       </c>
@@ -15664,11 +15901,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J31" s="1">
+        <f t="shared" si="16"/>
+        <v>83.2</v>
+      </c>
+      <c r="K31" s="1">
         <f t="shared" si="15"/>
-        <v>83.2</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="14"/>
         <v>39.619047619047628</v>
       </c>
     </row>
@@ -15679,7 +15916,7 @@
       <c r="C32" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -15695,17 +15932,17 @@
         <f>B33*1.35582</f>
         <v>1.35582</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="27"/>
+      <c r="E33" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
@@ -15714,7 +15951,7 @@
       <c r="C34" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="14"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="6" t="s">
         <v>52</v>
       </c>
@@ -15745,7 +15982,7 @@
         <f>B35*0.7457</f>
         <v>0.74570000000000003</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="8">
         <v>0</v>
       </c>
@@ -15765,12 +16002,12 @@
         <v>384</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" ref="K35:K44" si="16">H35*$J$35/$F$35</f>
+        <f t="shared" ref="K35:K44" si="17">H35*$J$35/$F$35</f>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D36" s="14"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="8">
         <v>500</v>
       </c>
@@ -15787,16 +16024,16 @@
         <v>0.94240837696335078</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" ref="J36:J44" si="17">F36*$J$35/$F$35</f>
+        <f t="shared" ref="J36:J44" si="18">F36*$J$35/$F$35</f>
         <v>384</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D37" s="14"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="8">
         <v>1000</v>
       </c>
@@ -15813,16 +16050,16 @@
         <v>1.8848167539267016</v>
       </c>
       <c r="J37" s="1">
+        <f t="shared" si="18"/>
+        <v>384</v>
+      </c>
+      <c r="K37" s="1">
         <f t="shared" si="17"/>
-        <v>384</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="16"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="14"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="8">
         <v>1500</v>
       </c>
@@ -15839,16 +16076,16 @@
         <v>2.8272251308900525</v>
       </c>
       <c r="J38" s="1">
+        <f t="shared" si="18"/>
+        <v>384</v>
+      </c>
+      <c r="K38" s="1">
         <f t="shared" si="17"/>
-        <v>384</v>
-      </c>
-      <c r="K38" s="1">
-        <f t="shared" si="16"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="14"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="8">
         <v>2000</v>
       </c>
@@ -15865,16 +16102,16 @@
         <v>3.7696335078534031</v>
       </c>
       <c r="J39" s="1">
+        <f t="shared" si="18"/>
+        <v>384</v>
+      </c>
+      <c r="K39" s="1">
         <f t="shared" si="17"/>
-        <v>384</v>
-      </c>
-      <c r="K39" s="1">
-        <f t="shared" si="16"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="14"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="8">
         <v>2650</v>
       </c>
@@ -15891,16 +16128,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J40" s="1">
+        <f t="shared" si="18"/>
+        <v>289.81132075471697</v>
+      </c>
+      <c r="K40" s="1">
         <f t="shared" si="17"/>
-        <v>289.81132075471697</v>
-      </c>
-      <c r="K40" s="1">
-        <f t="shared" si="16"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="14"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="8">
         <v>3000</v>
       </c>
@@ -15917,16 +16154,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J41" s="1">
+        <f t="shared" si="18"/>
+        <v>256</v>
+      </c>
+      <c r="K41" s="1">
         <f t="shared" si="17"/>
-        <v>256</v>
-      </c>
-      <c r="K41" s="1">
-        <f t="shared" si="16"/>
         <v>105.26896551724138</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="14"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="8">
         <v>3500</v>
       </c>
@@ -15943,16 +16180,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J42" s="1">
+        <f t="shared" si="18"/>
+        <v>219.42857142857147</v>
+      </c>
+      <c r="K42" s="1">
         <f t="shared" si="17"/>
-        <v>219.42857142857147</v>
-      </c>
-      <c r="K42" s="1">
-        <f t="shared" si="16"/>
         <v>90.23054187192119</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="14"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="8">
         <v>4000</v>
       </c>
@@ -15969,16 +16206,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J43" s="1">
+        <f t="shared" si="18"/>
+        <v>192</v>
+      </c>
+      <c r="K43" s="1">
         <f t="shared" si="17"/>
-        <v>192</v>
-      </c>
-      <c r="K43" s="1">
-        <f t="shared" si="16"/>
         <v>78.951724137931052</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D44" s="14"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="8">
         <v>4500</v>
       </c>
@@ -15995,11 +16232,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J44" s="1">
+        <f t="shared" si="18"/>
+        <v>170.66666666666669</v>
+      </c>
+      <c r="K44" s="1">
         <f t="shared" si="17"/>
-        <v>170.66666666666669</v>
-      </c>
-      <c r="K44" s="1">
-        <f t="shared" si="16"/>
         <v>70.179310344827584</v>
       </c>
     </row>
@@ -16012,16 +16249,16 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
     </row>
     <row r="47" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="E47" s="6" t="s">
@@ -16067,7 +16304,7 @@
         <v>638</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" ref="K48:K60" si="18">H48*$J$48/$F$48</f>
+        <f t="shared" ref="K48:K60" si="19">H48*$J$48/$F$48</f>
         <v>239.25</v>
       </c>
     </row>
@@ -16088,11 +16325,11 @@
         <v>1.5706806282722514</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" ref="J49:J60" si="19">F49*$J$48/$F$48</f>
+        <f t="shared" ref="J49:J60" si="20">F49*$J$48/$F$48</f>
         <v>638</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16113,11 +16350,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J50" s="1">
+        <f t="shared" si="20"/>
+        <v>638</v>
+      </c>
+      <c r="K50" s="1">
         <f t="shared" si="19"/>
-        <v>638</v>
-      </c>
-      <c r="K50" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16138,11 +16375,11 @@
         <v>4.7120418848167542</v>
       </c>
       <c r="J51" s="1">
+        <f t="shared" si="20"/>
+        <v>638</v>
+      </c>
+      <c r="K51" s="1">
         <f t="shared" si="19"/>
-        <v>638</v>
-      </c>
-      <c r="K51" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16163,11 +16400,11 @@
         <v>6.2827225130890056</v>
       </c>
       <c r="J52" s="1">
+        <f t="shared" si="20"/>
+        <v>638</v>
+      </c>
+      <c r="K52" s="1">
         <f t="shared" si="19"/>
-        <v>638</v>
-      </c>
-      <c r="K52" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16188,11 +16425,11 @@
         <v>7.5392670157068062</v>
       </c>
       <c r="J53" s="1">
+        <f t="shared" si="20"/>
+        <v>638</v>
+      </c>
+      <c r="K53" s="1">
         <f t="shared" si="19"/>
-        <v>638</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16213,11 +16450,11 @@
         <v>8.167539267015707</v>
       </c>
       <c r="J54" s="1">
+        <f t="shared" si="20"/>
+        <v>588.92307692307691</v>
+      </c>
+      <c r="K54" s="1">
         <f t="shared" si="19"/>
-        <v>588.92307692307691</v>
-      </c>
-      <c r="K54" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16238,11 +16475,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J55" s="1">
+        <f t="shared" si="20"/>
+        <v>483.02839116719241</v>
+      </c>
+      <c r="K55" s="1">
         <f t="shared" si="19"/>
-        <v>483.02839116719241</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="18"/>
         <v>239.25</v>
       </c>
     </row>
@@ -16263,11 +16500,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J56" s="1">
+        <f t="shared" si="20"/>
+        <v>382.8</v>
+      </c>
+      <c r="K56" s="1">
         <f t="shared" si="19"/>
-        <v>382.8</v>
-      </c>
-      <c r="K56" s="1">
-        <f t="shared" si="18"/>
         <v>189.60562499999997</v>
       </c>
     </row>
@@ -16288,11 +16525,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J57" s="1">
+        <f t="shared" si="20"/>
+        <v>340.26666666666665</v>
+      </c>
+      <c r="K57" s="1">
         <f t="shared" si="19"/>
-        <v>340.26666666666665</v>
-      </c>
-      <c r="K57" s="1">
-        <f t="shared" si="18"/>
         <v>168.53833333333333</v>
       </c>
     </row>
@@ -16313,11 +16550,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J58" s="1">
+        <f t="shared" si="20"/>
+        <v>306.24</v>
+      </c>
+      <c r="K58" s="1">
         <f t="shared" si="19"/>
-        <v>306.24</v>
-      </c>
-      <c r="K58" s="1">
-        <f t="shared" si="18"/>
         <v>151.68450000000001</v>
       </c>
     </row>
@@ -16338,11 +16575,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J59" s="1">
+        <f t="shared" si="20"/>
+        <v>278.39999999999998</v>
+      </c>
+      <c r="K59" s="1">
         <f t="shared" si="19"/>
-        <v>278.39999999999998</v>
-      </c>
-      <c r="K59" s="1">
-        <f t="shared" si="18"/>
         <v>137.89499999999998</v>
       </c>
     </row>
@@ -16363,25 +16600,25 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J60" s="1">
+        <f t="shared" si="20"/>
+        <v>255.2</v>
+      </c>
+      <c r="K60" s="1">
         <f t="shared" si="19"/>
-        <v>255.2</v>
-      </c>
-      <c r="K60" s="1">
-        <f t="shared" si="18"/>
         <v>126.40374999999999</v>
       </c>
     </row>
     <row r="62" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
     </row>
     <row r="63" spans="5:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E63" s="6" t="s">
@@ -16693,16 +16930,16 @@
       <c r="K79" s="1"/>
     </row>
     <row r="81" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E81" s="13" t="s">
+      <c r="E81" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
     </row>
     <row r="82" spans="5:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E82" s="6" t="s">
@@ -17193,16 +17430,16 @@
       <c r="J108" s="1"/>
     </row>
     <row r="111" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E111" s="13" t="s">
+      <c r="E111" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="26"/>
     </row>
     <row r="112" spans="5:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E112" s="6" t="s">
@@ -17513,16 +17750,16 @@
       <c r="J128" s="1"/>
     </row>
     <row r="131" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E131" s="13" t="s">
+      <c r="E131" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="13"/>
+      <c r="F131" s="26"/>
+      <c r="G131" s="26"/>
+      <c r="H131" s="26"/>
+      <c r="I131" s="26"/>
+      <c r="J131" s="26"/>
+      <c r="K131" s="26"/>
+      <c r="L131" s="26"/>
     </row>
     <row r="132" spans="5:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E132" s="6" t="s">
@@ -17849,7 +18086,659 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05C09A9-CE96-4D11-BF33-EA09C13CA751}">
+  <dimension ref="A1:K39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="32">
+        <v>15000</v>
+      </c>
+      <c r="C2" s="32">
+        <v>300</v>
+      </c>
+      <c r="D2" s="32">
+        <v>1330</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1.35</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="32">
+        <v>4000</v>
+      </c>
+      <c r="I2" s="32">
+        <v>125</v>
+      </c>
+      <c r="J2" s="32">
+        <v>250</v>
+      </c>
+      <c r="K2" s="22">
+        <v>35.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="20">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="23">
+        <v>47.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="14">
+        <v>5000</v>
+      </c>
+      <c r="I4" s="14">
+        <v>250</v>
+      </c>
+      <c r="J4" s="14">
+        <v>500</v>
+      </c>
+      <c r="K4" s="24">
+        <v>52.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="20">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="14">
+        <v>5000</v>
+      </c>
+      <c r="I5" s="14">
+        <v>450</v>
+      </c>
+      <c r="J5" s="14">
+        <v>900</v>
+      </c>
+      <c r="K5" s="24">
+        <v>57.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="21">
+        <v>4.43</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="32">
+        <v>1106</v>
+      </c>
+      <c r="I6" s="32">
+        <v>500</v>
+      </c>
+      <c r="J6" s="32">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="22">
+        <v>21.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="37">
+        <v>15000</v>
+      </c>
+      <c r="C7" s="37">
+        <v>300</v>
+      </c>
+      <c r="D7" s="37">
+        <v>4000</v>
+      </c>
+      <c r="E7" s="19">
+        <v>5.2</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="25">
+        <v>30.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="20">
+        <v>6.04</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="25">
+        <v>45.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="20">
+        <v>7.04</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="23">
+        <v>50.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="20">
+        <v>8.08</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="32">
+        <v>5000</v>
+      </c>
+      <c r="I10" s="32">
+        <v>3500</v>
+      </c>
+      <c r="J10" s="32">
+        <v>7000</v>
+      </c>
+      <c r="K10" s="22">
+        <v>18.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="20">
+        <v>9.1</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="25">
+        <v>24.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="20">
+        <v>10.11</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="25">
+        <v>25.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="20">
+        <v>11.05</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="25">
+        <v>47.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="20">
+        <v>11.9</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="25">
+        <v>57.49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="21">
+        <v>13.35</v>
+      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="23">
+        <v>64.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="37">
+        <v>12000</v>
+      </c>
+      <c r="C16" s="37">
+        <v>600</v>
+      </c>
+      <c r="D16" s="37">
+        <v>2100</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="20">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="20">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="21">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="37">
+        <v>12000</v>
+      </c>
+      <c r="C20" s="37">
+        <v>600</v>
+      </c>
+      <c r="D20" s="37">
+        <v>6500</v>
+      </c>
+      <c r="E20" s="19">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="20">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="20">
+        <v>8.5500000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="20">
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="20">
+        <v>9.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="20">
+        <v>10.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="39"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="20">
+        <v>12.36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="36"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="21">
+        <v>13.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="37">
+        <v>7500</v>
+      </c>
+      <c r="C28" s="37">
+        <v>1200</v>
+      </c>
+      <c r="D28" s="37">
+        <v>4770</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="20">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="21">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37">
+        <v>265</v>
+      </c>
+      <c r="D33" s="37"/>
+      <c r="E33" s="19">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="20">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="21">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="37">
+        <v>12500</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="19">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="37">
+        <v>12500</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="19">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="36"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="21">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63d68cde8d91d9cfd93ef1e7c2dce69f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490d39c642ce3fbaaaf8418555bb1ddb" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -18066,22 +18955,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08470758-3E41-49AE-BF09-F8ECFDDA61D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18100,19 +18988,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating with Peak torque data
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnigear.sharepoint.com/sites/Engineering/Shared Documents/Electrification/Customer_Related/JLG/60FT_Boom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{0D9695E0-4620-4509-9A87-EB14C5946FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3BD2B62E-7697-4D2E-9A98-1D3D452C6CFB}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{0D9695E0-4620-4509-9A87-EB14C5946FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CF16564D-DEB0-41E3-A321-36BD19C1BDC6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
+    <workbookView xWindow="2790" yWindow="240" windowWidth="32820" windowHeight="20415" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -2786,7 +2786,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Acc+Application!$U$2:$U$10</c:v>
+            <c:v>Acc</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -16519,7 +16519,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{95D0F4A2-D7A5-4DAF-9BFA-7435D72E787A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="170" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="164" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16530,16 +16530,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>395286</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442911</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17087,7 +17087,7 @@
   <dimension ref="A1:U150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG49" sqref="AG49"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated time stamp, need to add M34
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnigear.sharepoint.com/sites/Engineering/Shared Documents/Electrification/Customer_Related/TrovaCV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ElectricMotors\Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{B96C6DE6-D80B-45EE-A17B-89420AD46C4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{39F182C3-0817-48F9-901E-E9D73C7012DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA98FF66-6BE2-48D6-91EB-40BD2C03B266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="132">
   <si>
     <t>Value</t>
   </si>
@@ -431,6 +431,9 @@
   <si>
     <t>Max Speed on Max Grade</t>
   </si>
+  <si>
+    <t>Time Step</t>
+  </si>
 </sst>
 </file>
 
@@ -439,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,8 +466,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,8 +512,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -627,11 +643,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -723,13 +755,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -741,26 +782,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1023,6 +1060,57 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Application!$V$2:$V$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Application!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
@@ -1031,94 +1119,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Application!$V$2:$V$15</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.528</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25.056000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>37.584000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50.112000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>62.639999999999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>75.168000000000006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79.92</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>79.92</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.5999999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.88</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1185,7 +1222,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Application!$E$2:$E$15</c:f>
+              <c:f>Application!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1193,43 +1230,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,7 +1305,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -1280,7 +1317,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1344,11 +1381,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>time</a:t>
+                  <a:t>vehicle</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> [s]</a:t>
+                  <a:t> speed [km/hr] </a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1424,6 +1461,7 @@
         <c:axId val="967380448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1461,8 +1499,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>vehicle speed [Km/hr]</a:t>
+                  <a:t>time</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1653,6 +1696,36 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2700,22 +2773,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.02788021603192</c:v>
+                  <c:v>1120.7217013977379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950.0557604320638</c:v>
+                  <c:v>2241.4434027954758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2925.0836406480958</c:v>
+                  <c:v>3362.1651041932137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3900.1115208641277</c:v>
+                  <c:v>4482.8868055909516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4875.1394010801596</c:v>
+                  <c:v>5603.6085069886894</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5850.1672812961915</c:v>
+                  <c:v>6220.0054427574451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6220.0054427574451</c:v>
@@ -2733,31 +2806,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.872512690355329</c:v>
+                  <c:v>43.415474619289341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339.43435452382886</c:v>
+                  <c:v>296.82506446700512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.6064645057578</c:v>
+                  <c:v>298.373630964467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342.55998114230596</c:v>
+                  <c:v>300.95457512690353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>345.29490443347362</c:v>
+                  <c:v>304.56789695431473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.81123437926021</c:v>
+                  <c:v>309.21359644670048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>353.10897097966648</c:v>
+                  <c:v>198.40675169035529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.49250622262511</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.772419203045683</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2827,7 +2900,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>540.74238868672023</c:v>
+                  <c:v>1258.9259594020218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2894,7 +2967,7 @@
                   <c:v>224.14434027954755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.09021267471724</c:v>
+                  <c:v>84.054127604830342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2906,16 +2979,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>104.81730048432841</c:v>
+                  <c:v>353.21397416696402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.8213029225783</c:v>
+                  <c:v>660.37530049042368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>373.28710450929304</c:v>
+                  <c:v>1258.9466069230596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>540.75045410496602</c:v>
+                  <c:v>1258.9288629319428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4970,22 +5043,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.02788021603192</c:v>
+                  <c:v>1120.7217013977379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950.0557604320638</c:v>
+                  <c:v>2241.4434027954758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2925.0836406480958</c:v>
+                  <c:v>3362.1651041932137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3900.1115208641277</c:v>
+                  <c:v>4482.8868055909516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4875.1394010801596</c:v>
+                  <c:v>5603.6085069886894</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5850.1672812961915</c:v>
+                  <c:v>6220.0054427574451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6220.0054427574451</c:v>
@@ -5003,31 +5076,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.872512690355329</c:v>
+                  <c:v>43.415474619289341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339.43435452382886</c:v>
+                  <c:v>296.82506446700512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.6064645057578</c:v>
+                  <c:v>298.373630964467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342.55998114230596</c:v>
+                  <c:v>300.95457512690353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>345.29490443347362</c:v>
+                  <c:v>304.56789695431473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.81123437926021</c:v>
+                  <c:v>309.21359644670048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>353.10897097966648</c:v>
+                  <c:v>198.40675169035529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.49250622262511</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.772419203045683</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5101,7 +5174,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>540.74238868672023</c:v>
+                  <c:v>1258.9259594020218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5168,7 +5241,7 @@
                   <c:v>224.14434027954755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.09021267471724</c:v>
+                  <c:v>84.054127604830342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5180,16 +5253,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>104.81730048432841</c:v>
+                  <c:v>353.21397416696402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.8213029225783</c:v>
+                  <c:v>660.37530049042368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>373.28710450929304</c:v>
+                  <c:v>1258.9466069230596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>540.75045410496602</c:v>
+                  <c:v>1258.9288629319428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7728,22 +7801,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.02788021603192</c:v>
+                  <c:v>1120.7217013977379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950.0557604320638</c:v>
+                  <c:v>2241.4434027954758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2925.0836406480958</c:v>
+                  <c:v>3362.1651041932137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3900.1115208641277</c:v>
+                  <c:v>4482.8868055909516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4875.1394010801596</c:v>
+                  <c:v>5603.6085069886894</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5850.1672812961915</c:v>
+                  <c:v>6220.0054427574451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6220.0054427574451</c:v>
@@ -7761,31 +7834,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.872512690355329</c:v>
+                  <c:v>43.415474619289341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339.43435452382886</c:v>
+                  <c:v>296.82506446700512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.6064645057578</c:v>
+                  <c:v>298.373630964467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342.55998114230596</c:v>
+                  <c:v>300.95457512690353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>345.29490443347362</c:v>
+                  <c:v>304.56789695431473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.81123437926021</c:v>
+                  <c:v>309.21359644670048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>353.10897097966648</c:v>
+                  <c:v>198.40675169035529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.49250622262511</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.772419203045683</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7859,7 +7932,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>540.74238868672023</c:v>
+                  <c:v>1258.9259594020218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7926,7 +7999,7 @@
                   <c:v>224.14434027954755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.09021267471724</c:v>
+                  <c:v>84.054127604830342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7938,16 +8011,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>104.81730048432841</c:v>
+                  <c:v>353.21397416696402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.8213029225783</c:v>
+                  <c:v>660.37530049042368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>373.28710450929304</c:v>
+                  <c:v>1258.9466069230596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>540.75045410496602</c:v>
+                  <c:v>1258.9288629319428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10044,22 +10117,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.02788021603192</c:v>
+                  <c:v>1120.7217013977379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950.0557604320638</c:v>
+                  <c:v>2241.4434027954758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2925.0836406480958</c:v>
+                  <c:v>3362.1651041932137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3900.1115208641277</c:v>
+                  <c:v>4482.8868055909516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4875.1394010801596</c:v>
+                  <c:v>5603.6085069886894</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5850.1672812961915</c:v>
+                  <c:v>6220.0054427574451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6220.0054427574451</c:v>
@@ -10077,31 +10150,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.872512690355329</c:v>
+                  <c:v>43.415474619289341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339.43435452382886</c:v>
+                  <c:v>296.82506446700512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.6064645057578</c:v>
+                  <c:v>298.373630964467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342.55998114230596</c:v>
+                  <c:v>300.95457512690353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>345.29490443347362</c:v>
+                  <c:v>304.56789695431473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.81123437926021</c:v>
+                  <c:v>309.21359644670048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>353.10897097966648</c:v>
+                  <c:v>198.40675169035529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.49250622262511</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.772419203045683</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10171,7 +10244,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>540.74238868672023</c:v>
+                  <c:v>1258.9259594020218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10238,7 +10311,7 @@
                   <c:v>224.14434027954755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.09021267471724</c:v>
+                  <c:v>84.054127604830342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10250,16 +10323,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>104.81730048432841</c:v>
+                  <c:v>353.21397416696402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.8213029225783</c:v>
+                  <c:v>660.37530049042368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>373.28710450929304</c:v>
+                  <c:v>1258.9466069230596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>540.75045410496602</c:v>
+                  <c:v>1258.9288629319428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12204,22 +12277,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.02788021603192</c:v>
+                  <c:v>1120.7217013977379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950.0557604320638</c:v>
+                  <c:v>2241.4434027954758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2925.0836406480958</c:v>
+                  <c:v>3362.1651041932137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3900.1115208641277</c:v>
+                  <c:v>4482.8868055909516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4875.1394010801596</c:v>
+                  <c:v>5603.6085069886894</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5850.1672812961915</c:v>
+                  <c:v>6220.0054427574451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6220.0054427574451</c:v>
@@ -12237,31 +12310,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.872512690355329</c:v>
+                  <c:v>43.415474619289341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339.43435452382886</c:v>
+                  <c:v>296.82506446700512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.6064645057578</c:v>
+                  <c:v>298.373630964467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342.55998114230596</c:v>
+                  <c:v>300.95457512690353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>345.29490443347362</c:v>
+                  <c:v>304.56789695431473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.81123437926021</c:v>
+                  <c:v>309.21359644670048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>353.10897097966648</c:v>
+                  <c:v>198.40675169035529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.49250622262511</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.772419203045683</c:v>
+                  <c:v>59.315381131979699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12331,7 +12404,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>540.74238868672023</c:v>
+                  <c:v>1258.9259594020218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12398,7 +12471,7 @@
                   <c:v>224.14434027954755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.09021267471724</c:v>
+                  <c:v>84.054127604830342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12410,16 +12483,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>104.81730048432841</c:v>
+                  <c:v>353.21397416696402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.8213029225783</c:v>
+                  <c:v>660.37530049042368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>373.28710450929304</c:v>
+                  <c:v>1258.9466069230596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>540.75045410496602</c:v>
+                  <c:v>1258.9288629319428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15892,10 +15965,10 @@
       <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16428,7 +16501,7 @@
   <dimension ref="A1:V150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16514,7 +16587,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="26">
-        <v>11000</v>
+        <v>37100</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>2</v>
@@ -16527,7 +16600,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="20">
-        <f>IF(F2&gt;$B$15,$B$15,F2)</f>
+        <f t="shared" ref="G2:G10" si="0">IF(F2&gt;$B$15,$B$15,F2)</f>
         <v>0</v>
       </c>
       <c r="H2" s="21">
@@ -16535,7 +16608,7 @@
       </c>
       <c r="I2" s="20">
         <f>$B$2*$B$3*$B$8</f>
-        <v>43164</v>
+        <v>145580.4</v>
       </c>
       <c r="J2" s="20">
         <v>0</v>
@@ -16549,7 +16622,7 @@
       </c>
       <c r="M2" s="20">
         <f>$B$2*$B$3*$B$7*COS(K2)</f>
-        <v>755.37</v>
+        <v>2547.6570000000002</v>
       </c>
       <c r="N2" s="20">
         <f>0.5*$B$5*$B$6*$B$4*G2^2</f>
@@ -16561,23 +16634,23 @@
       </c>
       <c r="P2" s="20">
         <f>SUM(L2,M2,N2,O2)</f>
-        <v>755.37</v>
+        <v>2547.6570000000002</v>
       </c>
       <c r="Q2" s="20">
         <f>P2*$B$9</f>
-        <v>355.02389999999997</v>
+        <v>1197.39879</v>
       </c>
       <c r="R2" s="20">
         <f>G2*60/2/PI()/$B$9</f>
         <v>0</v>
       </c>
       <c r="S2" s="20">
-        <f>$B$17*$B$18</f>
+        <f t="shared" ref="S2:S15" si="1">$B$17*$B$18</f>
         <v>13.79</v>
       </c>
       <c r="T2" s="20">
-        <f>Q2/S2/$B$16</f>
-        <v>12.872512690355329</v>
+        <f t="shared" ref="T2:T15" si="2">Q2/S2/$B$16</f>
+        <v>43.415474619289341</v>
       </c>
       <c r="U2" s="20">
         <f>R2*S2</f>
@@ -16600,23 +16673,24 @@
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="20">
-        <v>2</v>
+        <f>E2+$B$40</f>
+        <v>10</v>
       </c>
       <c r="F3" s="20">
-        <f>F2+$B$14*2</f>
-        <v>3.48</v>
+        <f>F2+$B$14*(E3-E2)</f>
+        <v>4</v>
       </c>
       <c r="G3" s="20">
-        <f>IF(F3&gt;$B$15,$B$15,F3)</f>
-        <v>3.48</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="H3" s="21">
         <f>(G3-G2)/(E3-E2)</f>
-        <v>1.74</v>
+        <v>0.4</v>
       </c>
       <c r="I3" s="20">
         <f>$I$2/G3</f>
-        <v>12403.448275862069</v>
+        <v>36395.1</v>
       </c>
       <c r="J3" s="20">
         <v>0</v>
@@ -16625,48 +16699,48 @@
         <v>0</v>
       </c>
       <c r="L3" s="20">
-        <f t="shared" ref="L3:L15" si="0">$B$2*$B$3*SIN(K3)</f>
+        <f t="shared" ref="L3:L15" si="3">$B$2*$B$3*SIN(K3)</f>
         <v>0</v>
       </c>
       <c r="M3" s="20">
-        <f t="shared" ref="M3:M15" si="1">$B$2*$B$3*$B$7*COS(K3)</f>
-        <v>755.37</v>
+        <f t="shared" ref="M3:M15" si="4">$B$2*$B$3*$B$7*COS(K3)</f>
+        <v>2547.6570000000002</v>
       </c>
       <c r="N3" s="20">
-        <f t="shared" ref="N3:N15" si="2">0.5*$B$5*$B$6*$B$4*G3^2</f>
-        <v>22.926803760000002</v>
+        <f t="shared" ref="N3:N15" si="5">0.5*$B$5*$B$6*$B$4*G3^2</f>
+        <v>30.290400000000002</v>
       </c>
       <c r="O3" s="20">
-        <f t="shared" ref="O3:O15" si="3">$B$2*H3</f>
-        <v>19140</v>
+        <f t="shared" ref="O3:O15" si="6">$B$2*H3</f>
+        <v>14840</v>
       </c>
       <c r="P3" s="20">
-        <f t="shared" ref="P3:P15" si="4">SUM(L3,M3,N3,O3)</f>
-        <v>19918.29680376</v>
+        <f t="shared" ref="P3:P15" si="7">SUM(L3,M3,N3,O3)</f>
+        <v>17417.947400000001</v>
       </c>
       <c r="Q3" s="20">
-        <f t="shared" ref="Q3:Q15" si="5">P3*$B$9</f>
-        <v>9361.5994977671999</v>
+        <f t="shared" ref="Q3:Q15" si="8">P3*$B$9</f>
+        <v>8186.4352779999999</v>
       </c>
       <c r="R3" s="20">
-        <f t="shared" ref="R3:R15" si="6">G3*60/2/PI()/$B$9</f>
-        <v>70.70543003742074</v>
+        <f t="shared" ref="R3:R15" si="9">G3*60/2/PI()/$B$9</f>
+        <v>81.27060923841465</v>
       </c>
       <c r="S3" s="20">
-        <f>$B$17*$B$18</f>
+        <f t="shared" si="1"/>
         <v>13.79</v>
       </c>
       <c r="T3" s="20">
-        <f>Q3/S3/$B$16</f>
-        <v>339.43435452382886</v>
+        <f t="shared" si="2"/>
+        <v>296.82506446700512</v>
       </c>
       <c r="U3" s="20">
-        <f t="shared" ref="U3:U15" si="7">R3*S3</f>
-        <v>975.02788021603192</v>
+        <f t="shared" ref="U3:U15" si="10">R3*S3</f>
+        <v>1120.7217013977379</v>
       </c>
       <c r="V3" s="20">
-        <f t="shared" ref="V3:V15" si="8">3600*G3/1000</f>
-        <v>12.528</v>
+        <f t="shared" ref="V3:V15" si="11">3600*G3/1000</f>
+        <v>14.4</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -16681,23 +16755,24 @@
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="20">
-        <v>4</v>
+        <f t="shared" ref="E4:E15" si="12">E3+$B$40</f>
+        <v>20</v>
       </c>
       <c r="F4" s="20">
-        <f>F3+$B$14*2</f>
-        <v>6.96</v>
+        <f t="shared" ref="F4:F15" si="13">F3+$B$14*(E4-E3)</f>
+        <v>8</v>
       </c>
       <c r="G4" s="20">
-        <f>IF(F4&gt;$B$15,$B$15,F4)</f>
-        <v>6.96</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="H4" s="21">
-        <f t="shared" ref="H4:H10" si="9">(G4-G3)/(E4-E3)</f>
-        <v>1.74</v>
+        <f t="shared" ref="H4:H10" si="14">(G4-G3)/(E4-E3)</f>
+        <v>0.4</v>
       </c>
       <c r="I4" s="20">
         <f>$I$2/G4</f>
-        <v>6201.7241379310344</v>
+        <v>18197.55</v>
       </c>
       <c r="J4" s="20">
         <v>0</v>
@@ -16706,48 +16781,48 @@
         <v>0</v>
       </c>
       <c r="L4" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M4" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N4" s="20">
+        <f t="shared" si="5"/>
+        <v>121.16160000000001</v>
+      </c>
+      <c r="O4" s="20">
+        <f t="shared" si="6"/>
+        <v>14840</v>
+      </c>
+      <c r="P4" s="20">
+        <f t="shared" si="7"/>
+        <v>17508.818599999999</v>
+      </c>
+      <c r="Q4" s="20">
+        <f t="shared" si="8"/>
+        <v>8229.1447419999986</v>
+      </c>
+      <c r="R4" s="20">
+        <f t="shared" si="9"/>
+        <v>162.5412184768293</v>
+      </c>
+      <c r="S4" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N4" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T4" s="20">
         <f t="shared" si="2"/>
-        <v>91.707215040000008</v>
-      </c>
-      <c r="O4" s="20">
-        <f t="shared" si="3"/>
-        <v>19140</v>
-      </c>
-      <c r="P4" s="20">
-        <f t="shared" si="4"/>
-        <v>19987.077215040001</v>
-      </c>
-      <c r="Q4" s="20">
-        <f t="shared" si="5"/>
-        <v>9393.9262910687994</v>
-      </c>
-      <c r="R4" s="20">
-        <f t="shared" si="6"/>
-        <v>141.41086007484148</v>
-      </c>
-      <c r="S4" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T4" s="20">
-        <f>Q4/S4/$B$16</f>
-        <v>340.6064645057578</v>
+        <v>298.373630964467</v>
       </c>
       <c r="U4" s="20">
-        <f t="shared" si="7"/>
-        <v>1950.0557604320638</v>
+        <f t="shared" si="10"/>
+        <v>2241.4434027954758</v>
       </c>
       <c r="V4" s="20">
-        <f t="shared" si="8"/>
-        <v>25.056000000000001</v>
+        <f t="shared" si="11"/>
+        <v>28.8</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -16762,23 +16837,24 @@
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="20">
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>30</v>
       </c>
       <c r="F5" s="20">
-        <f>F4+$B$14*2</f>
-        <v>10.44</v>
+        <f t="shared" si="13"/>
+        <v>12</v>
       </c>
       <c r="G5" s="20">
-        <f>IF(F5&gt;$B$15,$B$15,F5)</f>
-        <v>10.44</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="H5" s="21">
-        <f t="shared" si="9"/>
-        <v>1.7399999999999998</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="I5" s="20">
-        <f t="shared" ref="I5:I15" si="10">$I$2/G5</f>
-        <v>4134.4827586206902</v>
+        <f t="shared" ref="I5:I15" si="15">$I$2/G5</f>
+        <v>12131.699999999999</v>
       </c>
       <c r="J5" s="20">
         <v>0</v>
@@ -16787,48 +16863,48 @@
         <v>0</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M5" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N5" s="20">
+        <f t="shared" si="5"/>
+        <v>272.61360000000002</v>
+      </c>
+      <c r="O5" s="20">
+        <f t="shared" si="6"/>
+        <v>14840</v>
+      </c>
+      <c r="P5" s="20">
+        <f t="shared" si="7"/>
+        <v>17660.2706</v>
+      </c>
+      <c r="Q5" s="20">
+        <f t="shared" si="8"/>
+        <v>8300.3271819999991</v>
+      </c>
+      <c r="R5" s="20">
+        <f t="shared" si="9"/>
+        <v>243.81182771524394</v>
+      </c>
+      <c r="S5" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N5" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T5" s="20">
         <f t="shared" si="2"/>
-        <v>206.34123383999997</v>
-      </c>
-      <c r="O5" s="20">
-        <f t="shared" si="3"/>
-        <v>19139.999999999996</v>
-      </c>
-      <c r="P5" s="20">
-        <f t="shared" si="4"/>
-        <v>20101.711233839997</v>
-      </c>
-      <c r="Q5" s="20">
-        <f t="shared" si="5"/>
-        <v>9447.804279904798</v>
-      </c>
-      <c r="R5" s="20">
-        <f t="shared" si="6"/>
-        <v>212.11629011226222</v>
-      </c>
-      <c r="S5" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T5" s="20">
-        <f>Q5/S5/$B$16</f>
-        <v>342.55998114230596</v>
+        <v>300.95457512690353</v>
       </c>
       <c r="U5" s="20">
-        <f t="shared" si="7"/>
-        <v>2925.0836406480958</v>
+        <f t="shared" si="10"/>
+        <v>3362.1651041932137</v>
       </c>
       <c r="V5" s="20">
-        <f t="shared" si="8"/>
-        <v>37.584000000000003</v>
+        <f t="shared" si="11"/>
+        <v>43.2</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -16841,23 +16917,24 @@
       <c r="C6" s="26"/>
       <c r="D6" s="37"/>
       <c r="E6" s="20">
-        <v>8</v>
+        <f t="shared" si="12"/>
+        <v>40</v>
       </c>
       <c r="F6" s="20">
-        <f>F5+$B$14*2</f>
-        <v>13.92</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="G6" s="20">
-        <f>IF(F6&gt;$B$15,$B$15,F6)</f>
-        <v>13.92</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="H6" s="21">
-        <f t="shared" si="9"/>
-        <v>1.7400000000000002</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="I6" s="20">
-        <f t="shared" si="10"/>
-        <v>3100.8620689655172</v>
+        <f t="shared" si="15"/>
+        <v>9098.7749999999996</v>
       </c>
       <c r="J6" s="20">
         <v>0</v>
@@ -16866,48 +16943,48 @@
         <v>0</v>
       </c>
       <c r="L6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M6" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N6" s="20">
+        <f t="shared" si="5"/>
+        <v>484.64640000000003</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="6"/>
+        <v>14840</v>
+      </c>
+      <c r="P6" s="20">
+        <f t="shared" si="7"/>
+        <v>17872.303400000001</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="8"/>
+        <v>8399.9825980000005</v>
+      </c>
+      <c r="R6" s="20">
+        <f t="shared" si="9"/>
+        <v>325.0824369536586</v>
+      </c>
+      <c r="S6" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N6" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T6" s="20">
         <f t="shared" si="2"/>
-        <v>366.82886016000003</v>
-      </c>
-      <c r="O6" s="20">
-        <f t="shared" si="3"/>
-        <v>19140.000000000004</v>
-      </c>
-      <c r="P6" s="20">
-        <f t="shared" si="4"/>
-        <v>20262.198860160002</v>
-      </c>
-      <c r="Q6" s="20">
-        <f t="shared" si="5"/>
-        <v>9523.2334642752012</v>
-      </c>
-      <c r="R6" s="20">
-        <f t="shared" si="6"/>
-        <v>282.82172014968296</v>
-      </c>
-      <c r="S6" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T6" s="20">
-        <f>Q6/S6/$B$16</f>
-        <v>345.29490443347362</v>
+        <v>304.56789695431473</v>
       </c>
       <c r="U6" s="20">
-        <f t="shared" si="7"/>
-        <v>3900.1115208641277</v>
+        <f t="shared" si="10"/>
+        <v>4482.8868055909516</v>
       </c>
       <c r="V6" s="20">
-        <f t="shared" si="8"/>
-        <v>50.112000000000002</v>
+        <f t="shared" si="11"/>
+        <v>57.6</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -16920,23 +16997,24 @@
       <c r="C7" s="26"/>
       <c r="D7" s="37"/>
       <c r="E7" s="20">
-        <v>10</v>
+        <f t="shared" si="12"/>
+        <v>50</v>
       </c>
       <c r="F7" s="20">
-        <f>F6+$B$14*2</f>
-        <v>17.399999999999999</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="G7" s="20">
-        <f>IF(F7&gt;$B$15,$B$15,F7)</f>
-        <v>17.399999999999999</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="H7" s="21">
-        <f t="shared" si="9"/>
-        <v>1.7399999999999993</v>
+        <f t="shared" si="14"/>
+        <v>0.4</v>
       </c>
       <c r="I7" s="20">
-        <f t="shared" si="10"/>
-        <v>2480.6896551724139</v>
+        <f t="shared" si="15"/>
+        <v>7279.0199999999995</v>
       </c>
       <c r="J7" s="20">
         <v>0</v>
@@ -16945,48 +17023,48 @@
         <v>0</v>
       </c>
       <c r="L7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M7" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N7" s="20">
+        <f t="shared" si="5"/>
+        <v>757.26</v>
+      </c>
+      <c r="O7" s="20">
+        <f t="shared" si="6"/>
+        <v>14840</v>
+      </c>
+      <c r="P7" s="20">
+        <f t="shared" si="7"/>
+        <v>18144.917000000001</v>
+      </c>
+      <c r="Q7" s="20">
+        <f t="shared" si="8"/>
+        <v>8528.1109899999992</v>
+      </c>
+      <c r="R7" s="20">
+        <f t="shared" si="9"/>
+        <v>406.35304619207324</v>
+      </c>
+      <c r="S7" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N7" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T7" s="20">
         <f t="shared" si="2"/>
-        <v>573.17009399999995</v>
-      </c>
-      <c r="O7" s="20">
-        <f t="shared" si="3"/>
-        <v>19139.999999999993</v>
-      </c>
-      <c r="P7" s="20">
-        <f t="shared" si="4"/>
-        <v>20468.540093999993</v>
-      </c>
-      <c r="Q7" s="20">
-        <f t="shared" si="5"/>
-        <v>9620.2138441799962</v>
-      </c>
-      <c r="R7" s="20">
-        <f t="shared" si="6"/>
-        <v>353.5271501871037</v>
-      </c>
-      <c r="S7" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T7" s="20">
-        <f>Q7/S7/$B$16</f>
-        <v>348.81123437926021</v>
+        <v>309.21359644670048</v>
       </c>
       <c r="U7" s="20">
-        <f t="shared" si="7"/>
-        <v>4875.1394010801596</v>
+        <f t="shared" si="10"/>
+        <v>5603.6085069886894</v>
       </c>
       <c r="V7" s="20">
-        <f t="shared" si="8"/>
-        <v>62.639999999999993</v>
+        <f t="shared" si="11"/>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -16999,23 +17077,24 @@
       <c r="C8" s="26"/>
       <c r="D8" s="37"/>
       <c r="E8" s="20">
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>60</v>
       </c>
       <c r="F8" s="20">
-        <f>F7+$B$14*2</f>
-        <v>20.88</v>
+        <f t="shared" si="13"/>
+        <v>24</v>
       </c>
       <c r="G8" s="20">
-        <f>IF(F8&gt;$B$15,$B$15,F8)</f>
-        <v>20.88</v>
+        <f t="shared" si="0"/>
+        <v>22.2</v>
       </c>
       <c r="H8" s="21">
-        <f t="shared" si="9"/>
-        <v>1.7400000000000002</v>
+        <f t="shared" si="14"/>
+        <v>0.21999999999999992</v>
       </c>
       <c r="I8" s="20">
-        <f t="shared" si="10"/>
-        <v>2067.2413793103451</v>
+        <f t="shared" si="15"/>
+        <v>6557.6756756756758</v>
       </c>
       <c r="J8" s="20">
         <v>0</v>
@@ -17024,48 +17103,48 @@
         <v>0</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M8" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N8" s="20">
+        <f t="shared" si="5"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="O8" s="20">
+        <f t="shared" si="6"/>
+        <v>8161.9999999999973</v>
+      </c>
+      <c r="P8" s="20">
+        <f t="shared" si="7"/>
+        <v>11642.677045999997</v>
+      </c>
+      <c r="Q8" s="20">
+        <f t="shared" si="8"/>
+        <v>5472.0582116199985</v>
+      </c>
+      <c r="R8" s="20">
+        <f t="shared" si="9"/>
+        <v>451.05188127320127</v>
+      </c>
+      <c r="S8" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N8" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T8" s="20">
         <f t="shared" si="2"/>
-        <v>825.36493535999989</v>
-      </c>
-      <c r="O8" s="20">
-        <f t="shared" si="3"/>
-        <v>19140.000000000004</v>
-      </c>
-      <c r="P8" s="20">
-        <f t="shared" si="4"/>
-        <v>20720.734935360004</v>
-      </c>
-      <c r="Q8" s="20">
-        <f t="shared" si="5"/>
-        <v>9738.7454196192011</v>
-      </c>
-      <c r="R8" s="20">
-        <f t="shared" si="6"/>
-        <v>424.23258022452444</v>
-      </c>
-      <c r="S8" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T8" s="20">
-        <f>Q8/S8/$B$16</f>
-        <v>353.10897097966648</v>
+        <v>198.40675169035529</v>
       </c>
       <c r="U8" s="20">
-        <f t="shared" si="7"/>
-        <v>5850.1672812961915</v>
+        <f t="shared" si="10"/>
+        <v>6220.0054427574451</v>
       </c>
       <c r="V8" s="20">
-        <f t="shared" si="8"/>
-        <v>75.168000000000006</v>
+        <f t="shared" si="11"/>
+        <v>79.92</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -17080,23 +17159,24 @@
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="20">
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>70</v>
       </c>
       <c r="F9" s="20">
-        <f>F8+$B$14*2</f>
-        <v>24.36</v>
+        <f t="shared" si="13"/>
+        <v>28</v>
       </c>
       <c r="G9" s="20">
-        <f>IF(F9&gt;$B$15,$B$15,F9)</f>
+        <f t="shared" si="0"/>
         <v>22.2</v>
       </c>
       <c r="H9" s="21">
-        <f t="shared" si="9"/>
-        <v>0.66000000000000014</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="I9" s="20">
-        <f t="shared" si="10"/>
-        <v>1944.3243243243244</v>
+        <f t="shared" si="15"/>
+        <v>6557.6756756756758</v>
       </c>
       <c r="J9" s="20">
         <v>0</v>
@@ -17105,47 +17185,47 @@
         <v>0</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M9" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N9" s="20">
+        <f t="shared" si="5"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="O9" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="20">
+        <f t="shared" si="7"/>
+        <v>3480.6770460000002</v>
+      </c>
+      <c r="Q9" s="20">
+        <f t="shared" si="8"/>
+        <v>1635.91821162</v>
+      </c>
+      <c r="R9" s="20">
+        <f t="shared" si="9"/>
+        <v>451.05188127320127</v>
+      </c>
+      <c r="S9" s="20">
         <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N9" s="20">
+        <v>13.79</v>
+      </c>
+      <c r="T9" s="20">
         <f t="shared" si="2"/>
-        <v>933.02004599999998</v>
-      </c>
-      <c r="O9" s="20">
-        <f t="shared" si="3"/>
-        <v>7260.0000000000018</v>
-      </c>
-      <c r="P9" s="20">
-        <f t="shared" si="4"/>
-        <v>8948.3900460000023</v>
-      </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="5"/>
-        <v>4205.7433216200006</v>
-      </c>
-      <c r="R9" s="20">
-        <f t="shared" si="6"/>
-        <v>451.05188127320127</v>
-      </c>
-      <c r="S9" s="20">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T9" s="20">
-        <f>Q9/S9/$B$16</f>
-        <v>152.49250622262511</v>
+        <v>59.315381131979699</v>
       </c>
       <c r="U9" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>6220.0054427574451</v>
       </c>
       <c r="V9" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>79.92</v>
       </c>
     </row>
@@ -17159,23 +17239,24 @@
       <c r="C10" s="26"/>
       <c r="D10" s="37"/>
       <c r="E10" s="20">
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>80</v>
       </c>
       <c r="F10" s="20">
-        <f>F9+$B$14*2</f>
-        <v>27.84</v>
+        <f t="shared" si="13"/>
+        <v>32</v>
       </c>
       <c r="G10" s="20">
-        <f>IF(F10&gt;$B$15,$B$15,F10)</f>
+        <f t="shared" si="0"/>
         <v>22.2</v>
       </c>
       <c r="H10" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I10" s="20">
-        <f t="shared" si="10"/>
-        <v>1944.3243243243244</v>
+        <f t="shared" si="15"/>
+        <v>6557.6756756756758</v>
       </c>
       <c r="J10" s="20">
         <v>0</v>
@@ -17184,47 +17265,47 @@
         <v>0</v>
       </c>
       <c r="L10" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="20">
-        <f t="shared" si="1"/>
-        <v>755.37</v>
-      </c>
-      <c r="N10" s="20">
-        <f t="shared" si="2"/>
-        <v>933.02004599999998</v>
-      </c>
-      <c r="O10" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="M10" s="20">
+        <f t="shared" si="4"/>
+        <v>2547.6570000000002</v>
+      </c>
+      <c r="N10" s="20">
+        <f t="shared" si="5"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="O10" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="P10" s="20">
-        <f t="shared" si="4"/>
-        <v>1688.390046</v>
+        <f t="shared" si="7"/>
+        <v>3480.6770460000002</v>
       </c>
       <c r="Q10" s="20">
-        <f t="shared" si="5"/>
-        <v>793.54332161999992</v>
+        <f t="shared" si="8"/>
+        <v>1635.91821162</v>
       </c>
       <c r="R10" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>451.05188127320127</v>
       </c>
       <c r="S10" s="20">
-        <f>$B$17*$B$18</f>
+        <f t="shared" si="1"/>
         <v>13.79</v>
       </c>
       <c r="T10" s="20">
-        <f>Q10/S10/$B$16</f>
-        <v>28.772419203045683</v>
+        <f t="shared" si="2"/>
+        <v>59.315381131979699</v>
       </c>
       <c r="U10" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>6220.0054427574451</v>
       </c>
       <c r="V10" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>79.92</v>
       </c>
     </row>
@@ -17233,18 +17314,19 @@
         <v>128</v>
       </c>
       <c r="B11" s="26">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="24">
-        <v>18</v>
+      <c r="E11" s="20">
+        <f t="shared" si="12"/>
+        <v>90</v>
       </c>
       <c r="F11" s="24">
-        <f>F10+$B$14*2</f>
-        <v>31.32</v>
+        <f t="shared" si="13"/>
+        <v>36</v>
       </c>
       <c r="G11" s="24">
         <v>1E-3</v>
@@ -17253,59 +17335,59 @@
         <v>0</v>
       </c>
       <c r="I11" s="24">
-        <f t="shared" si="10"/>
-        <v>43164000</v>
+        <f t="shared" si="15"/>
+        <v>145580400</v>
       </c>
       <c r="J11" s="24">
         <f>Table2[[#This Row],[Value]]</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K11" s="24">
         <f>ATAN2(100, J11)</f>
-        <v>0.2914567944778671</v>
+        <v>0.19739555984988078</v>
       </c>
       <c r="L11" s="24">
-        <f t="shared" si="0"/>
-        <v>31007.710331464335</v>
+        <f t="shared" si="3"/>
+        <v>71376.663499677219</v>
       </c>
       <c r="M11" s="24">
+        <f t="shared" si="4"/>
+        <v>2498.1832224887025</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="5"/>
+        <v>1.89315E-6</v>
+      </c>
+      <c r="O11" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <f t="shared" si="7"/>
+        <v>73874.846724059069</v>
+      </c>
+      <c r="Q11" s="24">
+        <f t="shared" si="8"/>
+        <v>34721.177960307759</v>
+      </c>
+      <c r="R11" s="24">
+        <f t="shared" si="9"/>
+        <v>2.0317652309603661E-2</v>
+      </c>
+      <c r="S11" s="24">
         <f t="shared" si="1"/>
-        <v>723.51324106750121</v>
-      </c>
-      <c r="N11" s="24">
+        <v>13.79</v>
+      </c>
+      <c r="T11" s="24">
         <f t="shared" si="2"/>
-        <v>1.89315E-6</v>
-      </c>
-      <c r="O11" s="24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
-        <f t="shared" si="4"/>
-        <v>31731.223574424985</v>
-      </c>
-      <c r="Q11" s="24">
-        <f t="shared" si="5"/>
-        <v>14913.675079979743</v>
-      </c>
-      <c r="R11" s="24">
-        <f t="shared" si="6"/>
-        <v>2.0317652309603661E-2</v>
-      </c>
-      <c r="S11" s="24">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T11" s="24">
-        <f>Q11/S11/$B$16</f>
-        <v>540.74238868672023</v>
+        <v>1258.9259594020218</v>
       </c>
       <c r="U11" s="24">
         <f>R11*S11</f>
         <v>0.28018042534943444</v>
       </c>
       <c r="V11" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
@@ -17314,18 +17396,19 @@
         <v>129</v>
       </c>
       <c r="B12" s="26">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="22">
-        <v>20</v>
+      <c r="E12" s="20">
+        <f t="shared" si="12"/>
+        <v>100</v>
       </c>
       <c r="F12" s="22">
-        <f>F11+$B$14*2</f>
-        <v>34.799999999999997</v>
+        <f t="shared" si="13"/>
+        <v>40</v>
       </c>
       <c r="G12" s="34">
         <v>2</v>
@@ -17334,58 +17417,58 @@
         <v>0</v>
       </c>
       <c r="I12" s="22">
-        <f t="shared" si="10"/>
-        <v>21582</v>
+        <f t="shared" si="15"/>
+        <v>72790.2</v>
       </c>
       <c r="J12" s="34">
         <v>5</v>
       </c>
       <c r="K12" s="22">
-        <f t="shared" ref="K12:K15" si="11">ATAN2(100, J12)</f>
+        <f t="shared" ref="K12:K15" si="16">ATAN2(100, J12)</f>
         <v>4.9958395721942765E-2</v>
       </c>
       <c r="L12" s="22">
-        <f t="shared" si="0"/>
-        <v>5388.7682444154116</v>
+        <f t="shared" si="3"/>
+        <v>18174.845624346526</v>
       </c>
       <c r="M12" s="22">
+        <f t="shared" si="4"/>
+        <v>2544.4783874085133</v>
+      </c>
+      <c r="N12" s="22">
+        <f t="shared" si="5"/>
+        <v>7.5726000000000004</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="22">
+        <f t="shared" si="7"/>
+        <v>20726.896611755037</v>
+      </c>
+      <c r="Q12" s="22">
+        <f t="shared" si="8"/>
+        <v>9741.6414075248667</v>
+      </c>
+      <c r="R12" s="22">
+        <f t="shared" si="9"/>
+        <v>40.635304619207325</v>
+      </c>
+      <c r="S12" s="22">
         <f t="shared" si="1"/>
-        <v>754.42755421815752</v>
-      </c>
-      <c r="N12" s="22">
+        <v>13.79</v>
+      </c>
+      <c r="T12" s="22">
         <f t="shared" si="2"/>
-        <v>7.5726000000000004</v>
-      </c>
-      <c r="O12" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="22">
-        <f t="shared" si="4"/>
-        <v>6150.7683986335696</v>
-      </c>
-      <c r="Q12" s="22">
-        <f t="shared" si="5"/>
-        <v>2890.8611473577776</v>
-      </c>
-      <c r="R12" s="22">
-        <f t="shared" si="6"/>
-        <v>40.635304619207325</v>
-      </c>
-      <c r="S12" s="22">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T12" s="22">
-        <f>Q12/S12/$B$16</f>
-        <v>104.81730048432841</v>
+        <v>353.21397416696402</v>
       </c>
       <c r="U12" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>560.36085069886894</v>
       </c>
       <c r="V12" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>7.2</v>
       </c>
     </row>
@@ -17394,18 +17477,19 @@
         <v>130</v>
       </c>
       <c r="B13" s="26">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="22">
-        <v>22</v>
+      <c r="E13" s="20">
+        <f t="shared" si="12"/>
+        <v>110</v>
       </c>
       <c r="F13" s="22">
-        <f>F12+$B$14*2</f>
-        <v>38.279999999999994</v>
+        <f t="shared" si="13"/>
+        <v>44</v>
       </c>
       <c r="G13" s="34">
         <v>1</v>
@@ -17414,58 +17498,58 @@
         <v>0</v>
       </c>
       <c r="I13" s="22">
-        <f t="shared" si="10"/>
-        <v>43164</v>
+        <f t="shared" si="15"/>
+        <v>145580.4</v>
       </c>
       <c r="J13" s="34">
         <v>10</v>
       </c>
       <c r="K13" s="22">
+        <f t="shared" si="16"/>
+        <v>9.9668652491162038E-2</v>
+      </c>
+      <c r="L13" s="22">
+        <f t="shared" si="3"/>
+        <v>36214.478041411581</v>
+      </c>
+      <c r="M13" s="22">
+        <f t="shared" si="4"/>
+        <v>2535.0134628988103</v>
+      </c>
+      <c r="N13" s="22">
+        <f t="shared" si="5"/>
+        <v>1.8931500000000001</v>
+      </c>
+      <c r="O13" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="22">
+        <f t="shared" si="7"/>
+        <v>38751.384654310394</v>
+      </c>
+      <c r="Q13" s="22">
+        <f t="shared" si="8"/>
+        <v>18213.150787525883</v>
+      </c>
+      <c r="R13" s="22">
+        <f t="shared" si="9"/>
+        <v>20.317652309603663</v>
+      </c>
+      <c r="S13" s="22">
+        <f t="shared" si="1"/>
+        <v>13.79</v>
+      </c>
+      <c r="T13" s="22">
+        <f t="shared" si="2"/>
+        <v>660.37530049042368</v>
+      </c>
+      <c r="U13" s="22">
+        <f t="shared" si="10"/>
+        <v>280.18042534943447</v>
+      </c>
+      <c r="V13" s="22">
         <f t="shared" si="11"/>
-        <v>9.9668652491162038E-2</v>
-      </c>
-      <c r="L13" s="22">
-        <f t="shared" si="0"/>
-        <v>10737.446319555995</v>
-      </c>
-      <c r="M13" s="22">
-        <f t="shared" si="1"/>
-        <v>751.62124236891952</v>
-      </c>
-      <c r="N13" s="22">
-        <f t="shared" si="2"/>
-        <v>1.8931500000000001</v>
-      </c>
-      <c r="O13" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="22">
-        <f t="shared" si="4"/>
-        <v>11490.960711924914</v>
-      </c>
-      <c r="Q13" s="22">
-        <f t="shared" si="5"/>
-        <v>5400.7515346047094</v>
-      </c>
-      <c r="R13" s="22">
-        <f t="shared" si="6"/>
-        <v>20.317652309603663</v>
-      </c>
-      <c r="S13" s="22">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T13" s="22">
-        <f>Q13/S13/$B$16</f>
-        <v>195.8213029225783</v>
-      </c>
-      <c r="U13" s="22">
-        <f t="shared" si="7"/>
-        <v>280.18042534943447</v>
-      </c>
-      <c r="V13" s="22">
-        <f t="shared" si="8"/>
         <v>3.6</v>
       </c>
     </row>
@@ -17474,18 +17558,19 @@
         <v>17</v>
       </c>
       <c r="B14" s="26">
-        <v>1.74</v>
+        <v>0.4</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="37"/>
-      <c r="E14" s="22">
-        <v>24</v>
+      <c r="E14" s="20">
+        <f t="shared" si="12"/>
+        <v>120</v>
       </c>
       <c r="F14" s="22">
-        <f>F13+$B$14*2</f>
-        <v>41.759999999999991</v>
+        <f t="shared" si="13"/>
+        <v>48</v>
       </c>
       <c r="G14" s="34">
         <v>0.8</v>
@@ -17494,58 +17579,58 @@
         <v>0</v>
       </c>
       <c r="I14" s="22">
-        <f t="shared" si="10"/>
-        <v>53955</v>
+        <f t="shared" si="15"/>
+        <v>181975.49999999997</v>
       </c>
       <c r="J14" s="34">
         <v>20</v>
       </c>
       <c r="K14" s="22">
+        <f t="shared" si="16"/>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="L14" s="22">
+        <f t="shared" si="3"/>
+        <v>71376.663499677219</v>
+      </c>
+      <c r="M14" s="22">
+        <f t="shared" si="4"/>
+        <v>2498.1832224887025</v>
+      </c>
+      <c r="N14" s="22">
+        <f t="shared" si="5"/>
+        <v>1.2116160000000002</v>
+      </c>
+      <c r="O14" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="22">
+        <f t="shared" si="7"/>
+        <v>73876.058338165923</v>
+      </c>
+      <c r="Q14" s="22">
+        <f t="shared" si="8"/>
+        <v>34721.747418937979</v>
+      </c>
+      <c r="R14" s="22">
+        <f t="shared" si="9"/>
+        <v>16.254121847682928</v>
+      </c>
+      <c r="S14" s="22">
+        <f t="shared" si="1"/>
+        <v>13.79</v>
+      </c>
+      <c r="T14" s="22">
+        <f t="shared" si="2"/>
+        <v>1258.9466069230596</v>
+      </c>
+      <c r="U14" s="22">
+        <f t="shared" si="10"/>
+        <v>224.14434027954755</v>
+      </c>
+      <c r="V14" s="22">
         <f t="shared" si="11"/>
-        <v>0.19739555984988078</v>
-      </c>
-      <c r="L14" s="22">
-        <f t="shared" si="0"/>
-        <v>21162.89214276144</v>
-      </c>
-      <c r="M14" s="22">
-        <f t="shared" si="1"/>
-        <v>740.70122499665035</v>
-      </c>
-      <c r="N14" s="22">
-        <f t="shared" si="2"/>
-        <v>1.2116160000000002</v>
-      </c>
-      <c r="O14" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="22">
-        <f t="shared" si="4"/>
-        <v>21904.804983758091</v>
-      </c>
-      <c r="Q14" s="22">
-        <f t="shared" si="5"/>
-        <v>10295.258342366302</v>
-      </c>
-      <c r="R14" s="22">
-        <f t="shared" si="6"/>
-        <v>16.254121847682928</v>
-      </c>
-      <c r="S14" s="22">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T14" s="22">
-        <f>Q14/S14/$B$16</f>
-        <v>373.28710450929304</v>
-      </c>
-      <c r="U14" s="22">
-        <f t="shared" si="7"/>
-        <v>224.14434027954755</v>
-      </c>
-      <c r="V14" s="22">
-        <f t="shared" si="8"/>
         <v>2.88</v>
       </c>
     </row>
@@ -17560,75 +17645,76 @@
         <v>19</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="E15" s="22">
-        <v>26</v>
+      <c r="E15" s="20">
+        <f t="shared" si="12"/>
+        <v>130</v>
       </c>
       <c r="F15" s="22">
-        <f>F14+$B$14*2</f>
-        <v>45.239999999999988</v>
+        <f t="shared" si="13"/>
+        <v>52</v>
       </c>
       <c r="G15" s="34">
         <f>B13</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H15" s="23">
         <v>0</v>
       </c>
       <c r="I15" s="22">
-        <f t="shared" si="10"/>
-        <v>86328</v>
+        <f t="shared" si="15"/>
+        <v>485268</v>
       </c>
       <c r="J15" s="34">
         <f>B12</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K15" s="22">
+        <f t="shared" si="16"/>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="L15" s="22">
+        <f t="shared" si="3"/>
+        <v>71376.663499677219</v>
+      </c>
+      <c r="M15" s="22">
+        <f t="shared" si="4"/>
+        <v>2498.1832224887025</v>
+      </c>
+      <c r="N15" s="22">
+        <f t="shared" si="5"/>
+        <v>0.17038349999999999</v>
+      </c>
+      <c r="O15" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="22">
+        <f t="shared" si="7"/>
+        <v>73875.017105665916</v>
+      </c>
+      <c r="Q15" s="22">
+        <f t="shared" si="8"/>
+        <v>34721.258039662978</v>
+      </c>
+      <c r="R15" s="22">
+        <f t="shared" si="9"/>
+        <v>6.0952956928810984</v>
+      </c>
+      <c r="S15" s="22">
+        <f t="shared" si="1"/>
+        <v>13.79</v>
+      </c>
+      <c r="T15" s="22">
+        <f t="shared" si="2"/>
+        <v>1258.9288629319428</v>
+      </c>
+      <c r="U15" s="22">
+        <f t="shared" si="10"/>
+        <v>84.054127604830342</v>
+      </c>
+      <c r="V15" s="22">
         <f t="shared" si="11"/>
-        <v>0.2914567944778671</v>
-      </c>
-      <c r="L15" s="22">
-        <f t="shared" si="0"/>
-        <v>31007.710331464335</v>
-      </c>
-      <c r="M15" s="22">
-        <f t="shared" si="1"/>
-        <v>723.51324106750121</v>
-      </c>
-      <c r="N15" s="22">
-        <f t="shared" si="2"/>
-        <v>0.47328750000000003</v>
-      </c>
-      <c r="O15" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="22">
-        <f t="shared" si="4"/>
-        <v>31731.696860031836</v>
-      </c>
-      <c r="Q15" s="22">
-        <f t="shared" si="5"/>
-        <v>14913.897524214963</v>
-      </c>
-      <c r="R15" s="22">
-        <f t="shared" si="6"/>
-        <v>10.158826154801831</v>
-      </c>
-      <c r="S15" s="22">
-        <f>$B$17*$B$18</f>
-        <v>13.79</v>
-      </c>
-      <c r="T15" s="22">
-        <f>Q15/S15/$B$16</f>
-        <v>540.75045410496602</v>
-      </c>
-      <c r="U15" s="22">
-        <f t="shared" si="7"/>
-        <v>140.09021267471724</v>
-      </c>
-      <c r="V15" s="22">
-        <f t="shared" si="8"/>
-        <v>1.8</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -17753,7 +17839,7 @@
         <v>208</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" ref="K22:K31" si="12">H22*$J$22/$F$22</f>
+        <f t="shared" ref="K22:K31" si="17">H22*$J$22/$F$22</f>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17784,7 +17870,7 @@
         <v>208</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17816,7 +17902,7 @@
         <v>208</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17847,7 +17933,7 @@
         <v>208</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17876,11 +17962,11 @@
         <v>2.5130890052356021</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" ref="J26:J31" si="13">F26*$J$22/$F$22</f>
+        <f t="shared" ref="J26:J31" si="18">F26*$J$22/$F$22</f>
         <v>187.2</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17908,11 +17994,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>149.76</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -17941,11 +18027,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>124.8</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>59.428571428571445</v>
       </c>
     </row>
@@ -17973,11 +18059,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>106.97142857142858</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>50.938775510204088</v>
       </c>
     </row>
@@ -18006,11 +18092,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>93.6</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>44.571428571428577</v>
       </c>
     </row>
@@ -18038,11 +18124,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>83.2</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>39.619047619047628</v>
       </c>
     </row>
@@ -18062,7 +18148,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
         <v>47</v>
       </c>
@@ -18081,7 +18167,7 @@
       <c r="K33" s="36"/>
       <c r="L33" s="36"/>
     </row>
-    <row r="34" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="31">
         <v>1</v>
       </c>
@@ -18112,7 +18198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" s="33" t="s">
         <v>17</v>
       </c>
@@ -18137,11 +18223,11 @@
         <v>384</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" ref="K35:K44" si="14">H35*$J$35/$F$35</f>
+        <f t="shared" ref="K35:K44" si="19">H35*$J$35/$F$35</f>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
         <v>85</v>
       </c>
@@ -18165,15 +18251,15 @@
         <v>0.94240837696335078</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" ref="J36:J44" si="15">F36*$J$35/$F$35</f>
+        <f t="shared" ref="J36:J44" si="20">F36*$J$35/$F$35</f>
         <v>384</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
         <v>86</v>
       </c>
@@ -18197,15 +18283,15 @@
         <v>1.8848167539267016</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>384</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="28" t="s">
         <v>5</v>
       </c>
@@ -18230,15 +18316,15 @@
         <v>2.8272251308900525</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>384</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="37"/>
       <c r="E39" s="5">
         <v>2000</v>
@@ -18256,15 +18342,24 @@
         <v>3.7696335078534031</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>384</v>
       </c>
       <c r="K39" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="52">
+        <v>10</v>
+      </c>
+      <c r="C40" s="51" t="s">
+        <v>86</v>
+      </c>
       <c r="D40" s="37"/>
       <c r="E40" s="5">
         <v>2650</v>
@@ -18282,15 +18377,15 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>289.81132075471697</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>119.17241379310344</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D41" s="37"/>
       <c r="E41" s="5">
         <v>3000</v>
@@ -18308,15 +18403,15 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>256</v>
       </c>
       <c r="K41" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>105.26896551724138</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D42" s="37"/>
       <c r="E42" s="5">
         <v>3500</v>
@@ -18334,15 +18429,15 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>219.42857142857147</v>
       </c>
       <c r="K42" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>90.23054187192119</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D43" s="37"/>
       <c r="E43" s="5">
         <v>4000</v>
@@ -18360,15 +18455,15 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>192</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>78.951724137931052</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D44" s="37"/>
       <c r="E44" s="5">
         <v>4500</v>
@@ -18386,15 +18481,15 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>170.66666666666669</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>70.179310344827584</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -18402,7 +18497,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E46" s="36" t="s">
         <v>59</v>
       </c>
@@ -18414,7 +18509,7 @@
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
     </row>
-    <row r="47" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
         <v>50</v>
       </c>
@@ -18437,7 +18532,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E48" s="5">
         <v>0</v>
       </c>
@@ -18458,7 +18553,7 @@
         <v>638</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" ref="K48:K60" si="16">H48*$J$48/$F$48</f>
+        <f t="shared" ref="K48:K60" si="21">H48*$J$48/$F$48</f>
         <v>239.25</v>
       </c>
     </row>
@@ -18479,11 +18574,11 @@
         <v>1.5706806282722514</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" ref="J49:J60" si="17">F49*$J$48/$F$48</f>
+        <f t="shared" ref="J49:J60" si="22">F49*$J$48/$F$48</f>
         <v>638</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18504,11 +18599,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>638</v>
       </c>
       <c r="K50" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18529,11 +18624,11 @@
         <v>4.7120418848167542</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>638</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18554,11 +18649,11 @@
         <v>6.2827225130890056</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>638</v>
       </c>
       <c r="K52" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18579,11 +18674,11 @@
         <v>7.5392670157068062</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>638</v>
       </c>
       <c r="K53" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18604,11 +18699,11 @@
         <v>8.167539267015707</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>588.92307692307691</v>
       </c>
       <c r="K54" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18629,11 +18724,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>483.02839116719241</v>
       </c>
       <c r="K55" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>239.25</v>
       </c>
     </row>
@@ -18654,11 +18749,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>382.8</v>
       </c>
       <c r="K56" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>189.60562499999997</v>
       </c>
     </row>
@@ -18679,11 +18774,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>340.26666666666665</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>168.53833333333333</v>
       </c>
     </row>
@@ -18704,11 +18799,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>306.24</v>
       </c>
       <c r="K58" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>151.68450000000001</v>
       </c>
     </row>
@@ -18729,11 +18824,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>278.39999999999998</v>
       </c>
       <c r="K59" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>137.89499999999998</v>
       </c>
     </row>
@@ -18754,11 +18849,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>255.2</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>126.40374999999999</v>
       </c>
     </row>
@@ -21249,31 +21344,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="45">
         <v>15000</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="45">
         <v>300</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="45">
         <v>1330</v>
       </c>
       <c r="E2" s="12">
         <v>1.35</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="45">
         <v>4000</v>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="45">
         <v>125</v>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="45">
         <v>250</v>
       </c>
       <c r="K2" s="15">
@@ -21281,26 +21376,26 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="16">
         <v>47.74</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="13">
         <v>3.5</v>
       </c>
@@ -21321,10 +21416,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="13">
         <v>4</v>
       </c>
@@ -21345,23 +21440,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="14">
         <v>4.43</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="45">
         <v>1106</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="45">
         <v>500</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="45">
         <v>1000</v>
       </c>
       <c r="K6" s="15">
@@ -21369,79 +21464,79 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="42">
         <v>15000</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="42">
         <v>300</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="42">
         <v>4000</v>
       </c>
       <c r="E7" s="12">
         <v>5.2</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="18">
         <v>30.68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="13">
         <v>6.04</v>
       </c>
-      <c r="G8" s="40"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
       <c r="K8" s="18">
         <v>45.13</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="13">
         <v>7.04</v>
       </c>
-      <c r="G9" s="41"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
       <c r="K9" s="16">
         <v>50.62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="13">
         <v>8.08</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="45">
         <v>5000</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="45">
         <v>3500</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="45">
         <v>7000</v>
       </c>
       <c r="K10" s="15">
@@ -21449,96 +21544,96 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="13">
         <v>9.1</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
       <c r="K11" s="18">
         <v>24.92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="13">
         <v>10.11</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="18">
         <v>25.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="13">
         <v>11.05</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="18">
         <v>47.6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="13">
         <v>11.9</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="18">
         <v>57.49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="14">
         <v>13.35</v>
       </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
       <c r="K15" s="16">
         <v>64.08</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="42">
         <v>12000</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="42">
         <v>600</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="42">
         <v>2100</v>
       </c>
       <c r="E16" s="12">
@@ -21546,43 +21641,43 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="13">
         <v>1.97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="13">
         <v>2.88</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="14">
         <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="42">
         <v>12000</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="42">
         <v>600</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="42">
         <v>6500</v>
       </c>
       <c r="E20" s="12">
@@ -21590,79 +21685,79 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="13">
         <v>7.42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="13">
         <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="13">
         <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="13">
         <v>9.94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="13">
         <v>10.79</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="13">
         <v>12.36</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="14">
         <v>13.32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28" s="42">
         <v>7500</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="42">
         <v>1200</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="42">
         <v>4770</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -21670,83 +21765,83 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
       <c r="E29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
       <c r="E30" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="13">
         <v>2.97</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
       <c r="E32" s="14">
         <v>3.94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47">
+      <c r="B33" s="42"/>
+      <c r="C33" s="42">
         <v>265</v>
       </c>
-      <c r="D33" s="47"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="12">
         <v>2.98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="13">
         <v>3.98</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="14">
         <v>6.03</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="47">
+      <c r="B36" s="42">
         <v>12500</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E36" s="12">
@@ -21754,25 +21849,25 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
       <c r="E37" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="47">
+      <c r="B38" s="42">
         <v>12500</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="D38" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="12">
@@ -21780,33 +21875,27 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
       <c r="E39" s="14">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="D7:D15"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -21823,17 +21912,23 @@
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B27"/>
     <mergeCell ref="C20:C27"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -21841,12 +21936,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22067,15 +22159,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22100,10 +22196,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added total kW command
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnigear.sharepoint.com/sites/Engineering/Shared Documents/Electrification/Customer_Related/TrovaCV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ElectricMotors\Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{3866E8CC-F120-4580-BB5C-0FAD16DD0AEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{33D09417-6CE8-4396-9E9D-DE66292ECF97}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838DF4F0-C78B-4A37-A7D7-AD785BCAB201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="145">
   <si>
     <t>Value</t>
   </si>
@@ -467,6 +467,12 @@
   <si>
     <t>Total kW</t>
   </si>
+  <si>
+    <t>Battery Voltage [V]</t>
+  </si>
+  <si>
+    <t>Battery Current [A]</t>
+  </si>
 </sst>
 </file>
 
@@ -786,19 +792,40 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="12" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -810,36 +837,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="12" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -19519,10 +19525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335F5D5-EBE0-44CD-9439-894D8E00CE51}">
-  <dimension ref="A1:X164"/>
+  <dimension ref="A1:Z164"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19536,7 +19542,7 @@
     <col min="23" max="23" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
@@ -19546,7 +19552,7 @@
       <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -19603,14 +19609,20 @@
       <c r="V1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="53" t="s">
+      <c r="W1" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="X1" s="37" t="s">
         <v>142</v>
       </c>
+      <c r="Y1" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z1" s="37" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
@@ -19620,19 +19632,19 @@
       <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="20">
         <v>0</v>
       </c>
       <c r="F2" s="20">
-        <f>3600*H2/1000</f>
+        <f t="shared" ref="F2:F15" si="0">3600*H2/1000</f>
         <v>0</v>
       </c>
       <c r="G2" s="20">
         <v>0</v>
       </c>
       <c r="H2" s="20">
-        <f t="shared" ref="H2:H10" si="0">IF(G2&gt;$B$15,$B$15,G2)</f>
+        <f t="shared" ref="H2:H10" si="1">IF(G2&gt;$B$15,$B$15,G2)</f>
         <v>0</v>
       </c>
       <c r="I2" s="21">
@@ -19677,7 +19689,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="20">
-        <f t="shared" ref="T2:T15" si="1">$B$17*$B$18</f>
+        <f t="shared" ref="T2:T15" si="2">$B$17*$B$18</f>
         <v>13.986999999999998</v>
       </c>
       <c r="U2" s="20">
@@ -19688,16 +19700,19 @@
         <f>S2*T2</f>
         <v>0</v>
       </c>
-      <c r="W2" s="56">
+      <c r="W2" s="40">
         <f>U2*V2*2*PI()/60/1000</f>
         <v>0</v>
       </c>
-      <c r="X2" s="56">
+      <c r="X2" s="40">
         <f>W2*$B$16</f>
         <v>0</v>
       </c>
+      <c r="Y2">
+        <v>600</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -19707,29 +19722,29 @@
       <c r="C3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="20">
         <f>E2+$B$40</f>
         <v>10</v>
       </c>
       <c r="F3" s="20">
-        <f>3600*H3/1000</f>
+        <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
       <c r="G3" s="20">
-        <f>G2+$B$14*(E3-E2)</f>
+        <f t="shared" ref="G3:G15" si="3">G2+$B$14*(E3-E2)</f>
         <v>4</v>
       </c>
       <c r="H3" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I3" s="21">
-        <f>(H3-H2)/(E3-E2)</f>
+        <f t="shared" ref="I3:I10" si="4">(H3-H2)/(E3-E2)</f>
         <v>0.4</v>
       </c>
       <c r="J3" s="20">
-        <f>$J$2/H3</f>
+        <f t="shared" ref="J3:J15" si="5">$J$2/H3</f>
         <v>10791</v>
       </c>
       <c r="K3" s="20">
@@ -19739,55 +19754,58 @@
         <v>0</v>
       </c>
       <c r="M3" s="20">
-        <f t="shared" ref="M3:M15" si="2">$B$2*$B$3*SIN(L3)</f>
+        <f t="shared" ref="M3:M15" si="6">$B$2*$B$3*SIN(L3)</f>
         <v>0</v>
       </c>
       <c r="N3" s="20">
-        <f t="shared" ref="N3:N15" si="3">$B$2*$B$3*$B$7*COS(L3)</f>
+        <f t="shared" ref="N3:N15" si="7">$B$2*$B$3*$B$7*COS(L3)</f>
         <v>755.37</v>
       </c>
       <c r="O3" s="20">
-        <f t="shared" ref="O3:O15" si="4">0.5*$B$5*$B$6*$B$4*H3^2</f>
+        <f t="shared" ref="O3:O15" si="8">0.5*$B$5*$B$6*$B$4*H3^2</f>
         <v>30.290400000000002</v>
       </c>
       <c r="P3" s="20">
-        <f t="shared" ref="P3:P15" si="5">$B$2*I3</f>
+        <f t="shared" ref="P3:P15" si="9">$B$2*I3</f>
         <v>4400</v>
       </c>
       <c r="Q3" s="20">
-        <f t="shared" ref="Q3:Q15" si="6">SUM(M3,N3,O3,P3)</f>
+        <f t="shared" ref="Q3:Q15" si="10">SUM(M3,N3,O3,P3)</f>
         <v>5185.6603999999998</v>
       </c>
       <c r="R3" s="20">
-        <f t="shared" ref="R3:R15" si="7">Q3*$B$9</f>
+        <f t="shared" ref="R3:R15" si="11">Q3*$B$9</f>
         <v>2437.2603879999997</v>
       </c>
       <c r="S3" s="20">
-        <f t="shared" ref="S3:S15" si="8">H3*60/2/PI()/$B$9</f>
+        <f t="shared" ref="S3:S15" si="12">H3*60/2/PI()/$B$9</f>
         <v>81.27060923841465</v>
       </c>
       <c r="T3" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U3" s="20">
-        <f t="shared" ref="U3:U15" si="9">R3/T3/$B$16/$B$10</f>
+        <f t="shared" ref="U3:U15" si="13">R3/T3/$B$16/$B$10</f>
         <v>91.711491046197025</v>
       </c>
       <c r="V3" s="20">
-        <f t="shared" ref="V3:V15" si="10">S3*T3</f>
+        <f t="shared" ref="V3:V15" si="14">S3*T3</f>
         <v>1136.7320114177055</v>
       </c>
-      <c r="W3" s="56">
-        <f t="shared" ref="W3:W15" si="11">U3*V3*2*PI()/60/1000</f>
+      <c r="W3" s="40">
+        <f t="shared" ref="W3:W15" si="15">U3*V3*2*PI()/60/1000</f>
         <v>10.91717978947368</v>
       </c>
-      <c r="X3" s="56">
-        <f t="shared" ref="X3:X15" si="12">W3*$B$16</f>
+      <c r="X3" s="40">
+        <f t="shared" ref="X3:X15" si="16">W3*$B$16</f>
         <v>21.83435957894736</v>
       </c>
+      <c r="Y3">
+        <v>600</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>13</v>
       </c>
@@ -19797,29 +19815,29 @@
       <c r="C4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="20">
-        <f t="shared" ref="E4:E15" si="13">E3+$B$40</f>
+        <f t="shared" ref="E4:E15" si="17">E3+$B$40</f>
         <v>20</v>
       </c>
       <c r="F4" s="20">
-        <f>3600*H4/1000</f>
+        <f t="shared" si="0"/>
         <v>28.8</v>
       </c>
       <c r="G4" s="20">
-        <f>G3+$B$14*(E4-E3)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H4" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I4" s="21">
-        <f>(H4-H3)/(E4-E3)</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="J4" s="20">
-        <f>$J$2/H4</f>
+        <f t="shared" si="5"/>
         <v>5395.5</v>
       </c>
       <c r="K4" s="20">
@@ -19829,55 +19847,58 @@
         <v>0</v>
       </c>
       <c r="M4" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O4" s="20">
+        <f t="shared" si="8"/>
+        <v>121.16160000000001</v>
+      </c>
+      <c r="P4" s="20">
+        <f t="shared" si="9"/>
+        <v>4400</v>
+      </c>
+      <c r="Q4" s="20">
+        <f t="shared" si="10"/>
+        <v>5276.5316000000003</v>
+      </c>
+      <c r="R4" s="20">
+        <f t="shared" si="11"/>
+        <v>2479.9698520000002</v>
+      </c>
+      <c r="S4" s="20">
+        <f t="shared" si="12"/>
+        <v>162.5412184768293</v>
+      </c>
+      <c r="T4" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O4" s="20">
-        <f t="shared" si="4"/>
-        <v>121.16160000000001</v>
-      </c>
-      <c r="P4" s="20">
-        <f t="shared" si="5"/>
-        <v>4400</v>
-      </c>
-      <c r="Q4" s="20">
-        <f t="shared" si="6"/>
-        <v>5276.5316000000003</v>
-      </c>
-      <c r="R4" s="20">
-        <f t="shared" si="7"/>
-        <v>2479.9698520000002</v>
-      </c>
-      <c r="S4" s="20">
-        <f t="shared" si="8"/>
-        <v>162.5412184768293</v>
-      </c>
-      <c r="T4" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U4" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>93.318602311168661</v>
       </c>
       <c r="V4" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2273.464022835411</v>
       </c>
-      <c r="W4" s="56">
-        <f t="shared" si="11"/>
+      <c r="W4" s="40">
+        <f t="shared" si="15"/>
         <v>22.216975157894737</v>
       </c>
-      <c r="X4" s="56">
-        <f t="shared" si="12"/>
+      <c r="X4" s="40">
+        <f t="shared" si="16"/>
         <v>44.433950315789474</v>
       </c>
+      <c r="Y4">
+        <v>600</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
@@ -19887,29 +19908,29 @@
       <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>30</v>
       </c>
       <c r="F5" s="20">
-        <f>3600*H5/1000</f>
+        <f t="shared" si="0"/>
         <v>43.2</v>
       </c>
       <c r="G5" s="20">
-        <f>G4+$B$14*(E5-E4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H5" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I5" s="21">
-        <f>(H5-H4)/(E5-E4)</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="J5" s="20">
-        <f>$J$2/H5</f>
+        <f t="shared" si="5"/>
         <v>3597</v>
       </c>
       <c r="K5" s="20">
@@ -19919,55 +19940,58 @@
         <v>0</v>
       </c>
       <c r="M5" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O5" s="20">
+        <f t="shared" si="8"/>
+        <v>272.61360000000002</v>
+      </c>
+      <c r="P5" s="20">
+        <f t="shared" si="9"/>
+        <v>4400</v>
+      </c>
+      <c r="Q5" s="20">
+        <f t="shared" si="10"/>
+        <v>5427.9835999999996</v>
+      </c>
+      <c r="R5" s="20">
+        <f t="shared" si="11"/>
+        <v>2551.1522919999998</v>
+      </c>
+      <c r="S5" s="20">
+        <f t="shared" si="12"/>
+        <v>243.81182771524394</v>
+      </c>
+      <c r="T5" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O5" s="20">
-        <f t="shared" si="4"/>
-        <v>272.61360000000002</v>
-      </c>
-      <c r="P5" s="20">
-        <f t="shared" si="5"/>
-        <v>4400</v>
-      </c>
-      <c r="Q5" s="20">
-        <f t="shared" si="6"/>
-        <v>5427.9835999999996</v>
-      </c>
-      <c r="R5" s="20">
-        <f t="shared" si="7"/>
-        <v>2551.1522919999998</v>
-      </c>
-      <c r="S5" s="20">
-        <f t="shared" si="8"/>
-        <v>243.81182771524394</v>
-      </c>
-      <c r="T5" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U5" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>95.997121086121339</v>
       </c>
       <c r="V5" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3410.1960342531165</v>
       </c>
-      <c r="W5" s="56">
-        <f t="shared" si="11"/>
+      <c r="W5" s="40">
+        <f t="shared" si="15"/>
         <v>34.282001684210528</v>
       </c>
-      <c r="X5" s="56">
-        <f t="shared" si="12"/>
+      <c r="X5" s="40">
+        <f t="shared" si="16"/>
         <v>68.564003368421055</v>
       </c>
+      <c r="Y5">
+        <v>600</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>15</v>
       </c>
@@ -19975,29 +19999,29 @@
         <v>0.75</v>
       </c>
       <c r="C6" s="26"/>
-      <c r="D6" s="38"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>40</v>
       </c>
       <c r="F6" s="20">
-        <f>3600*H6/1000</f>
+        <f t="shared" si="0"/>
         <v>57.6</v>
       </c>
       <c r="G6" s="20">
-        <f>G5+$B$14*(E6-E5)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="H6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="I6" s="21">
-        <f>(H6-H5)/(E6-E5)</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="J6" s="20">
-        <f>$J$2/H6</f>
+        <f t="shared" si="5"/>
         <v>2697.75</v>
       </c>
       <c r="K6" s="20">
@@ -20007,55 +20031,58 @@
         <v>0</v>
       </c>
       <c r="M6" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="8"/>
+        <v>484.64640000000003</v>
+      </c>
+      <c r="P6" s="20">
+        <f t="shared" si="9"/>
+        <v>4400</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="10"/>
+        <v>5640.0164000000004</v>
+      </c>
+      <c r="R6" s="20">
+        <f t="shared" si="11"/>
+        <v>2650.8077080000003</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="12"/>
+        <v>325.0824369536586</v>
+      </c>
+      <c r="T6" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O6" s="20">
-        <f t="shared" si="4"/>
-        <v>484.64640000000003</v>
-      </c>
-      <c r="P6" s="20">
-        <f t="shared" si="5"/>
-        <v>4400</v>
-      </c>
-      <c r="Q6" s="20">
-        <f t="shared" si="6"/>
-        <v>5640.0164000000004</v>
-      </c>
-      <c r="R6" s="20">
-        <f t="shared" si="7"/>
-        <v>2650.8077080000003</v>
-      </c>
-      <c r="S6" s="20">
-        <f t="shared" si="8"/>
-        <v>325.0824369536586</v>
-      </c>
-      <c r="T6" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U6" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>99.747047371055103</v>
       </c>
       <c r="V6" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>4546.928045670822</v>
       </c>
-      <c r="W6" s="56">
-        <f t="shared" si="11"/>
+      <c r="W6" s="40">
+        <f t="shared" si="15"/>
         <v>47.49487494736843</v>
       </c>
-      <c r="X6" s="56">
-        <f t="shared" si="12"/>
+      <c r="X6" s="40">
+        <f t="shared" si="16"/>
         <v>94.98974989473686</v>
       </c>
+      <c r="Y6">
+        <v>600</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>123</v>
       </c>
@@ -20063,29 +20090,29 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="C7" s="26"/>
-      <c r="D7" s="38"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>50</v>
       </c>
       <c r="F7" s="20">
-        <f>3600*H7/1000</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="G7" s="20">
-        <f>G6+$B$14*(E7-E6)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="H7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I7" s="21">
-        <f>(H7-H6)/(E7-E6)</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="J7" s="20">
-        <f>$J$2/H7</f>
+        <f t="shared" si="5"/>
         <v>2158.1999999999998</v>
       </c>
       <c r="K7" s="20">
@@ -20095,55 +20122,58 @@
         <v>0</v>
       </c>
       <c r="M7" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O7" s="20">
+        <f t="shared" si="8"/>
+        <v>757.26</v>
+      </c>
+      <c r="P7" s="20">
+        <f t="shared" si="9"/>
+        <v>4400</v>
+      </c>
+      <c r="Q7" s="20">
+        <f t="shared" si="10"/>
+        <v>5912.63</v>
+      </c>
+      <c r="R7" s="20">
+        <f t="shared" si="11"/>
+        <v>2778.9360999999999</v>
+      </c>
+      <c r="S7" s="20">
+        <f t="shared" si="12"/>
+        <v>406.35304619207324</v>
+      </c>
+      <c r="T7" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O7" s="20">
-        <f t="shared" si="4"/>
-        <v>757.26</v>
-      </c>
-      <c r="P7" s="20">
-        <f t="shared" si="5"/>
-        <v>4400</v>
-      </c>
-      <c r="Q7" s="20">
-        <f t="shared" si="6"/>
-        <v>5912.63</v>
-      </c>
-      <c r="R7" s="20">
-        <f t="shared" si="7"/>
-        <v>2778.9360999999999</v>
-      </c>
-      <c r="S7" s="20">
-        <f t="shared" si="8"/>
-        <v>406.35304619207324</v>
-      </c>
-      <c r="T7" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U7" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>104.56838116596991</v>
       </c>
       <c r="V7" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>5683.6600570885275</v>
       </c>
-      <c r="W7" s="56">
-        <f t="shared" si="11"/>
+      <c r="W7" s="40">
+        <f t="shared" si="15"/>
         <v>62.238210526315783</v>
       </c>
-      <c r="X7" s="56">
-        <f t="shared" si="12"/>
+      <c r="X7" s="40">
+        <f t="shared" si="16"/>
         <v>124.47642105263157</v>
       </c>
+      <c r="Y7">
+        <v>600</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
@@ -20151,29 +20181,29 @@
         <v>0.4</v>
       </c>
       <c r="C8" s="26"/>
-      <c r="D8" s="38"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>60</v>
       </c>
       <c r="F8" s="20">
-        <f>3600*H8/1000</f>
+        <f t="shared" si="0"/>
         <v>79.92</v>
       </c>
       <c r="G8" s="20">
-        <f>G7+$B$14*(E8-E7)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="H8" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
       <c r="I8" s="21">
-        <f>(H8-H7)/(E8-E7)</f>
+        <f t="shared" si="4"/>
         <v>0.21999999999999992</v>
       </c>
       <c r="J8" s="20">
-        <f>$J$2/H8</f>
+        <f t="shared" si="5"/>
         <v>1944.3243243243244</v>
       </c>
       <c r="K8" s="20">
@@ -20183,55 +20213,58 @@
         <v>0</v>
       </c>
       <c r="M8" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O8" s="20">
+        <f t="shared" si="8"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="P8" s="20">
+        <f t="shared" si="9"/>
+        <v>2419.9999999999991</v>
+      </c>
+      <c r="Q8" s="20">
+        <f t="shared" si="10"/>
+        <v>4108.3900459999986</v>
+      </c>
+      <c r="R8" s="20">
+        <f t="shared" si="11"/>
+        <v>1930.9433216199993</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="12"/>
+        <v>451.05188127320127</v>
+      </c>
+      <c r="T8" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O8" s="20">
-        <f t="shared" si="4"/>
-        <v>933.02004599999998</v>
-      </c>
-      <c r="P8" s="20">
-        <f t="shared" si="5"/>
-        <v>2419.9999999999991</v>
-      </c>
-      <c r="Q8" s="20">
-        <f t="shared" si="6"/>
-        <v>4108.3900459999986</v>
-      </c>
-      <c r="R8" s="20">
-        <f t="shared" si="7"/>
-        <v>1930.9433216199993</v>
-      </c>
-      <c r="S8" s="20">
-        <f t="shared" si="8"/>
-        <v>451.05188127320127</v>
-      </c>
-      <c r="T8" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U8" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>72.659323568125274</v>
       </c>
       <c r="V8" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6308.8626633682652</v>
       </c>
-      <c r="W8" s="56">
-        <f t="shared" si="11"/>
+      <c r="W8" s="40">
+        <f t="shared" si="15"/>
         <v>48.0032942216842</v>
       </c>
-      <c r="X8" s="56">
-        <f t="shared" si="12"/>
+      <c r="X8" s="40">
+        <f t="shared" si="16"/>
         <v>96.0065884433684</v>
       </c>
+      <c r="Y8">
+        <v>600</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
@@ -20241,29 +20274,29 @@
       <c r="C9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>70</v>
       </c>
       <c r="F9" s="20">
-        <f>3600*H9/1000</f>
+        <f t="shared" si="0"/>
         <v>79.92</v>
       </c>
       <c r="G9" s="20">
-        <f>G8+$B$14*(E9-E8)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="H9" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
       <c r="I9" s="21">
-        <f>(H9-H8)/(E9-E8)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J9" s="20">
-        <f>$J$2/H9</f>
+        <f t="shared" si="5"/>
         <v>1944.3243243243244</v>
       </c>
       <c r="K9" s="20">
@@ -20273,55 +20306,58 @@
         <v>0</v>
       </c>
       <c r="M9" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O9" s="20">
+        <f t="shared" si="8"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="P9" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="20">
+        <f t="shared" si="10"/>
+        <v>1688.390046</v>
+      </c>
+      <c r="R9" s="20">
+        <f t="shared" si="11"/>
+        <v>793.54332161999992</v>
+      </c>
+      <c r="S9" s="20">
+        <f t="shared" si="12"/>
+        <v>451.05188127320127</v>
+      </c>
+      <c r="T9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O9" s="20">
-        <f t="shared" si="4"/>
-        <v>933.02004599999998</v>
-      </c>
-      <c r="P9" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="6"/>
-        <v>1688.390046</v>
-      </c>
-      <c r="R9" s="20">
-        <f t="shared" si="7"/>
-        <v>793.54332161999992</v>
-      </c>
-      <c r="S9" s="20">
-        <f t="shared" si="8"/>
-        <v>451.05188127320127</v>
-      </c>
-      <c r="T9" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U9" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>29.860183012797599</v>
       </c>
       <c r="V9" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6308.8626633682652</v>
       </c>
-      <c r="W9" s="56">
-        <f t="shared" si="11"/>
+      <c r="W9" s="40">
+        <f t="shared" si="15"/>
         <v>19.727504747999998</v>
       </c>
-      <c r="X9" s="56">
-        <f t="shared" si="12"/>
+      <c r="X9" s="40">
+        <f t="shared" si="16"/>
         <v>39.455009495999995</v>
       </c>
+      <c r="Y9">
+        <v>600</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>12</v>
       </c>
@@ -20329,29 +20365,29 @@
         <v>0.95</v>
       </c>
       <c r="C10" s="26"/>
-      <c r="D10" s="38"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>80</v>
       </c>
       <c r="F10" s="20">
-        <f>3600*H10/1000</f>
+        <f t="shared" si="0"/>
         <v>79.92</v>
       </c>
       <c r="G10" s="20">
-        <f>G9+$B$14*(E10-E9)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
       <c r="I10" s="21">
-        <f>(H10-H9)/(E10-E9)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J10" s="20">
-        <f>$J$2/H10</f>
+        <f t="shared" si="5"/>
         <v>1944.3243243243244</v>
       </c>
       <c r="K10" s="20">
@@ -20361,55 +20397,58 @@
         <v>0</v>
       </c>
       <c r="M10" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="20">
+        <f t="shared" si="7"/>
+        <v>755.37</v>
+      </c>
+      <c r="O10" s="20">
+        <f t="shared" si="8"/>
+        <v>933.02004599999998</v>
+      </c>
+      <c r="P10" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="20">
+        <f t="shared" si="10"/>
+        <v>1688.390046</v>
+      </c>
+      <c r="R10" s="20">
+        <f t="shared" si="11"/>
+        <v>793.54332161999992</v>
+      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="12"/>
+        <v>451.05188127320127</v>
+      </c>
+      <c r="T10" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="20">
-        <f t="shared" si="3"/>
-        <v>755.37</v>
-      </c>
-      <c r="O10" s="20">
-        <f t="shared" si="4"/>
-        <v>933.02004599999998</v>
-      </c>
-      <c r="P10" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="20">
-        <f t="shared" si="6"/>
-        <v>1688.390046</v>
-      </c>
-      <c r="R10" s="20">
-        <f t="shared" si="7"/>
-        <v>793.54332161999992</v>
-      </c>
-      <c r="S10" s="20">
-        <f t="shared" si="8"/>
-        <v>451.05188127320127</v>
-      </c>
-      <c r="T10" s="20">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U10" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>29.860183012797599</v>
       </c>
       <c r="V10" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6308.8626633682652</v>
       </c>
-      <c r="W10" s="56">
-        <f t="shared" si="11"/>
+      <c r="W10" s="40">
+        <f t="shared" si="15"/>
         <v>19.727504747999998</v>
       </c>
-      <c r="X10" s="56">
-        <f t="shared" si="12"/>
+      <c r="X10" s="40">
+        <f t="shared" si="16"/>
         <v>39.455009495999995</v>
       </c>
+      <c r="Y10">
+        <v>600</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>128</v>
       </c>
@@ -20419,17 +20458,17 @@
       <c r="C11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>90</v>
       </c>
       <c r="F11" s="24">
-        <f>3600*H11/1000</f>
+        <f t="shared" si="0"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="G11" s="24">
-        <f>G10+$B$14*(E11-E10)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="H11" s="24">
@@ -20439,7 +20478,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="24">
-        <f>$J$2/H11</f>
+        <f t="shared" si="5"/>
         <v>43164000</v>
       </c>
       <c r="K11" s="24">
@@ -20451,55 +20490,58 @@
         <v>0.19739555984988078</v>
       </c>
       <c r="M11" s="24">
+        <f t="shared" si="6"/>
+        <v>21162.89214276144</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="7"/>
+        <v>740.70122499665035</v>
+      </c>
+      <c r="O11" s="24">
+        <f t="shared" si="8"/>
+        <v>1.89315E-6</v>
+      </c>
+      <c r="P11" s="24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="24">
+        <f t="shared" si="10"/>
+        <v>21903.59336965124</v>
+      </c>
+      <c r="R11" s="24">
+        <f t="shared" si="11"/>
+        <v>10294.688883736082</v>
+      </c>
+      <c r="S11" s="24">
+        <f t="shared" si="12"/>
+        <v>2.0317652309603661E-2</v>
+      </c>
+      <c r="T11" s="24">
         <f t="shared" si="2"/>
-        <v>21162.89214276144</v>
-      </c>
-      <c r="N11" s="24">
-        <f t="shared" si="3"/>
-        <v>740.70122499665035</v>
-      </c>
-      <c r="O11" s="24">
-        <f t="shared" si="4"/>
-        <v>1.89315E-6</v>
-      </c>
-      <c r="P11" s="24">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="24">
-        <f t="shared" si="6"/>
-        <v>21903.59336965124</v>
-      </c>
-      <c r="R11" s="24">
-        <f t="shared" si="7"/>
-        <v>10294.688883736082</v>
-      </c>
-      <c r="S11" s="24">
-        <f t="shared" si="8"/>
-        <v>2.0317652309603661E-2</v>
-      </c>
-      <c r="T11" s="24">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U11" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>387.37808731175505</v>
       </c>
       <c r="V11" s="24">
         <f>S11*T11</f>
         <v>0.28418300285442638</v>
       </c>
-      <c r="W11" s="54">
-        <f t="shared" si="11"/>
+      <c r="W11" s="38">
+        <f t="shared" si="15"/>
         <v>1.1528207036658548E-2</v>
       </c>
-      <c r="X11" s="54">
-        <f t="shared" si="12"/>
+      <c r="X11" s="38">
+        <f t="shared" si="16"/>
         <v>2.3056414073317096E-2</v>
       </c>
+      <c r="Y11">
+        <v>600</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>129</v>
       </c>
@@ -20509,17 +20551,17 @@
       <c r="C12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="38"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
       <c r="F12" s="22">
-        <f>3600*H12/1000</f>
+        <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
       <c r="G12" s="22">
-        <f>G11+$B$14*(E12-E11)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="H12" s="34">
@@ -20529,66 +20571,69 @@
         <v>0</v>
       </c>
       <c r="J12" s="22">
-        <f>$J$2/H12</f>
+        <f t="shared" si="5"/>
         <v>21582</v>
       </c>
       <c r="K12" s="34">
         <v>5</v>
       </c>
       <c r="L12" s="22">
-        <f t="shared" ref="L12:L15" si="14">ATAN2(100, K12)</f>
+        <f t="shared" ref="L12:L15" si="18">ATAN2(100, K12)</f>
         <v>4.9958395721942765E-2</v>
       </c>
       <c r="M12" s="22">
+        <f t="shared" si="6"/>
+        <v>5388.7682444154116</v>
+      </c>
+      <c r="N12" s="22">
+        <f t="shared" si="7"/>
+        <v>754.42755421815752</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="8"/>
+        <v>7.5726000000000004</v>
+      </c>
+      <c r="P12" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="22">
+        <f t="shared" si="10"/>
+        <v>6150.7683986335696</v>
+      </c>
+      <c r="R12" s="22">
+        <f t="shared" si="11"/>
+        <v>2890.8611473577776</v>
+      </c>
+      <c r="S12" s="22">
+        <f t="shared" si="12"/>
+        <v>40.635304619207325</v>
+      </c>
+      <c r="T12" s="22">
         <f t="shared" si="2"/>
-        <v>5388.7682444154116</v>
-      </c>
-      <c r="N12" s="22">
-        <f t="shared" si="3"/>
-        <v>754.42755421815752</v>
-      </c>
-      <c r="O12" s="22">
-        <f t="shared" si="4"/>
-        <v>7.5726000000000004</v>
-      </c>
-      <c r="P12" s="22">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="22">
-        <f t="shared" si="6"/>
-        <v>6150.7683986335696</v>
-      </c>
-      <c r="R12" s="22">
-        <f t="shared" si="7"/>
-        <v>2890.8611473577776</v>
-      </c>
-      <c r="S12" s="22">
-        <f t="shared" si="8"/>
-        <v>40.635304619207325</v>
-      </c>
-      <c r="T12" s="22">
-        <f t="shared" si="1"/>
         <v>13.986999999999998</v>
       </c>
       <c r="U12" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>108.78000050263884</v>
       </c>
       <c r="V12" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>568.36600570885275</v>
       </c>
-      <c r="W12" s="55">
-        <f t="shared" si="11"/>
+      <c r="W12" s="39">
+        <f t="shared" si="15"/>
         <v>6.4744930511932317</v>
       </c>
-      <c r="X12" s="55">
-        <f t="shared" si="12"/>
+      <c r="X12" s="39">
+        <f t="shared" si="16"/>
         <v>12.948986102386463</v>
       </c>
+      <c r="Y12">
+        <v>600</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>130</v>
       </c>
@@ -20598,17 +20643,17 @@
       <c r="C13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>110</v>
       </c>
       <c r="F13" s="22">
-        <f>3600*H13/1000</f>
+        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
       <c r="G13" s="22">
-        <f>G12+$B$14*(E13-E12)</f>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="H13" s="34">
@@ -20618,66 +20663,69 @@
         <v>0</v>
       </c>
       <c r="J13" s="22">
-        <f>$J$2/H13</f>
+        <f t="shared" si="5"/>
         <v>43164</v>
       </c>
       <c r="K13" s="34">
         <v>10</v>
       </c>
       <c r="L13" s="22">
+        <f t="shared" si="18"/>
+        <v>9.9668652491162038E-2</v>
+      </c>
+      <c r="M13" s="22">
+        <f t="shared" si="6"/>
+        <v>10737.446319555995</v>
+      </c>
+      <c r="N13" s="22">
+        <f t="shared" si="7"/>
+        <v>751.62124236891952</v>
+      </c>
+      <c r="O13" s="22">
+        <f t="shared" si="8"/>
+        <v>1.8931500000000001</v>
+      </c>
+      <c r="P13" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="22">
+        <f t="shared" si="10"/>
+        <v>11490.960711924914</v>
+      </c>
+      <c r="R13" s="22">
+        <f t="shared" si="11"/>
+        <v>5400.7515346047094</v>
+      </c>
+      <c r="S13" s="22">
+        <f t="shared" si="12"/>
+        <v>20.317652309603663</v>
+      </c>
+      <c r="T13" s="22">
+        <f t="shared" si="2"/>
+        <v>13.986999999999998</v>
+      </c>
+      <c r="U13" s="22">
+        <f t="shared" si="13"/>
+        <v>203.22448042372844</v>
+      </c>
+      <c r="V13" s="22">
         <f t="shared" si="14"/>
-        <v>9.9668652491162038E-2</v>
-      </c>
-      <c r="M13" s="22">
-        <f t="shared" si="2"/>
-        <v>10737.446319555995</v>
-      </c>
-      <c r="N13" s="22">
-        <f t="shared" si="3"/>
-        <v>751.62124236891952</v>
-      </c>
-      <c r="O13" s="22">
-        <f t="shared" si="4"/>
-        <v>1.8931500000000001</v>
-      </c>
-      <c r="P13" s="22">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="22">
-        <f t="shared" si="6"/>
-        <v>11490.960711924914</v>
-      </c>
-      <c r="R13" s="22">
-        <f t="shared" si="7"/>
-        <v>5400.7515346047094</v>
-      </c>
-      <c r="S13" s="22">
-        <f t="shared" si="8"/>
-        <v>20.317652309603663</v>
-      </c>
-      <c r="T13" s="22">
-        <f t="shared" si="1"/>
-        <v>13.986999999999998</v>
-      </c>
-      <c r="U13" s="22">
-        <f t="shared" si="9"/>
-        <v>203.22448042372844</v>
-      </c>
-      <c r="V13" s="22">
-        <f t="shared" si="10"/>
         <v>284.18300285442638</v>
       </c>
-      <c r="W13" s="55">
-        <f t="shared" si="11"/>
+      <c r="W13" s="39">
+        <f t="shared" si="15"/>
         <v>6.0478740589078495</v>
       </c>
-      <c r="X13" s="55">
-        <f t="shared" si="12"/>
+      <c r="X13" s="39">
+        <f t="shared" si="16"/>
         <v>12.095748117815699</v>
       </c>
+      <c r="Y13">
+        <v>600</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>17</v>
       </c>
@@ -20687,17 +20735,17 @@
       <c r="C14" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>120</v>
       </c>
       <c r="F14" s="22">
-        <f>3600*H14/1000</f>
+        <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
       <c r="G14" s="22">
-        <f>G13+$B$14*(E14-E13)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="H14" s="34">
@@ -20707,66 +20755,69 @@
         <v>0</v>
       </c>
       <c r="J14" s="22">
-        <f>$J$2/H14</f>
+        <f t="shared" si="5"/>
         <v>53955</v>
       </c>
       <c r="K14" s="34">
         <v>20</v>
       </c>
       <c r="L14" s="22">
+        <f t="shared" si="18"/>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="M14" s="22">
+        <f t="shared" si="6"/>
+        <v>21162.89214276144</v>
+      </c>
+      <c r="N14" s="22">
+        <f t="shared" si="7"/>
+        <v>740.70122499665035</v>
+      </c>
+      <c r="O14" s="22">
+        <f t="shared" si="8"/>
+        <v>1.2116160000000002</v>
+      </c>
+      <c r="P14" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="22">
+        <f t="shared" si="10"/>
+        <v>21904.804983758091</v>
+      </c>
+      <c r="R14" s="22">
+        <f t="shared" si="11"/>
+        <v>10295.258342366302</v>
+      </c>
+      <c r="S14" s="22">
+        <f t="shared" si="12"/>
+        <v>16.254121847682928</v>
+      </c>
+      <c r="T14" s="22">
+        <f t="shared" si="2"/>
+        <v>13.986999999999998</v>
+      </c>
+      <c r="U14" s="22">
+        <f t="shared" si="13"/>
+        <v>387.39951542847319</v>
+      </c>
+      <c r="V14" s="22">
         <f t="shared" si="14"/>
-        <v>0.19739555984988078</v>
-      </c>
-      <c r="M14" s="22">
-        <f t="shared" si="2"/>
-        <v>21162.89214276144</v>
-      </c>
-      <c r="N14" s="22">
-        <f t="shared" si="3"/>
-        <v>740.70122499665035</v>
-      </c>
-      <c r="O14" s="22">
-        <f t="shared" si="4"/>
-        <v>1.2116160000000002</v>
-      </c>
-      <c r="P14" s="22">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="22">
-        <f t="shared" si="6"/>
-        <v>21904.804983758091</v>
-      </c>
-      <c r="R14" s="22">
-        <f t="shared" si="7"/>
-        <v>10295.258342366302</v>
-      </c>
-      <c r="S14" s="22">
-        <f t="shared" si="8"/>
-        <v>16.254121847682928</v>
-      </c>
-      <c r="T14" s="22">
-        <f t="shared" si="1"/>
-        <v>13.986999999999998</v>
-      </c>
-      <c r="U14" s="22">
-        <f t="shared" si="9"/>
-        <v>387.39951542847319</v>
-      </c>
-      <c r="V14" s="22">
-        <f t="shared" si="10"/>
         <v>227.3464022835411</v>
       </c>
-      <c r="W14" s="55">
-        <f t="shared" si="11"/>
+      <c r="W14" s="39">
+        <f t="shared" si="15"/>
         <v>9.2230757826349858</v>
       </c>
-      <c r="X14" s="55">
-        <f t="shared" si="12"/>
+      <c r="X14" s="39">
+        <f t="shared" si="16"/>
         <v>18.446151565269972</v>
       </c>
+      <c r="Y14">
+        <v>600</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>18</v>
       </c>
@@ -20776,17 +20827,17 @@
       <c r="C15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>130</v>
       </c>
       <c r="F15" s="22">
-        <f>3600*H15/1000</f>
+        <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
       <c r="G15" s="22">
-        <f>G14+$B$14*(E15-E14)</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="H15" s="34">
@@ -20797,7 +20848,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="22">
-        <f>$J$2/H15</f>
+        <f t="shared" si="5"/>
         <v>143880</v>
       </c>
       <c r="K15" s="34">
@@ -20805,59 +20856,62 @@
         <v>20</v>
       </c>
       <c r="L15" s="22">
+        <f t="shared" si="18"/>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="M15" s="22">
+        <f t="shared" si="6"/>
+        <v>21162.89214276144</v>
+      </c>
+      <c r="N15" s="22">
+        <f t="shared" si="7"/>
+        <v>740.70122499665035</v>
+      </c>
+      <c r="O15" s="22">
+        <f t="shared" si="8"/>
+        <v>0.17038349999999999</v>
+      </c>
+      <c r="P15" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="22">
+        <f t="shared" si="10"/>
+        <v>21903.763751258091</v>
+      </c>
+      <c r="R15" s="22">
+        <f t="shared" si="11"/>
+        <v>10294.768963091303</v>
+      </c>
+      <c r="S15" s="22">
+        <f t="shared" si="12"/>
+        <v>6.0952956928810984</v>
+      </c>
+      <c r="T15" s="22">
+        <f t="shared" si="2"/>
+        <v>13.986999999999998</v>
+      </c>
+      <c r="U15" s="22">
+        <f t="shared" si="13"/>
+        <v>387.38110061189542</v>
+      </c>
+      <c r="V15" s="22">
         <f t="shared" si="14"/>
-        <v>0.19739555984988078</v>
-      </c>
-      <c r="M15" s="22">
-        <f t="shared" si="2"/>
-        <v>21162.89214276144</v>
-      </c>
-      <c r="N15" s="22">
-        <f t="shared" si="3"/>
-        <v>740.70122499665035</v>
-      </c>
-      <c r="O15" s="22">
-        <f t="shared" si="4"/>
-        <v>0.17038349999999999</v>
-      </c>
-      <c r="P15" s="22">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="22">
-        <f t="shared" si="6"/>
-        <v>21903.763751258091</v>
-      </c>
-      <c r="R15" s="22">
-        <f t="shared" si="7"/>
-        <v>10294.768963091303</v>
-      </c>
-      <c r="S15" s="22">
-        <f t="shared" si="8"/>
-        <v>6.0952956928810984</v>
-      </c>
-      <c r="T15" s="22">
-        <f t="shared" si="1"/>
-        <v>13.986999999999998</v>
-      </c>
-      <c r="U15" s="22">
-        <f t="shared" si="9"/>
-        <v>387.38110061189542</v>
-      </c>
-      <c r="V15" s="22">
-        <f t="shared" si="10"/>
         <v>85.254900856327907</v>
       </c>
-      <c r="W15" s="55">
-        <f t="shared" si="11"/>
+      <c r="W15" s="39">
+        <f t="shared" si="15"/>
         <v>3.4584890133565409</v>
       </c>
-      <c r="X15" s="55">
-        <f t="shared" si="12"/>
+      <c r="X15" s="39">
+        <f t="shared" si="16"/>
         <v>6.9169780267130818</v>
       </c>
+      <c r="Y15">
+        <v>600</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>32</v>
       </c>
@@ -20865,7 +20919,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="26"/>
-      <c r="D16" s="38"/>
+      <c r="D16" s="43"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="S16" s="1"/>
@@ -20878,7 +20932,7 @@
         <v>3.94</v>
       </c>
       <c r="C17" s="26"/>
-      <c r="D17" s="38"/>
+      <c r="D17" s="43"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
@@ -20890,15 +20944,15 @@
         <v>3.55</v>
       </c>
       <c r="C18" s="26"/>
-      <c r="D18" s="38"/>
+      <c r="D18" s="43"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
@@ -20908,17 +20962,17 @@
       <c r="C20" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="51" t="s">
+      <c r="D20" s="43"/>
+      <c r="E20" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
     </row>
     <row r="21" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -20928,7 +20982,7 @@
       <c r="C21" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="2" t="s">
         <v>50</v>
       </c>
@@ -20959,7 +21013,7 @@
         <f>B22*0.453592</f>
         <v>29483.48</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="5">
         <v>0</v>
       </c>
@@ -20979,7 +21033,7 @@
         <v>208</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" ref="K22:K31" si="15">H22*$J$22/$F$22</f>
+        <f t="shared" ref="K22:K31" si="19">H22*$J$22/$F$22</f>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -20990,7 +21044,7 @@
       <c r="C23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="5">
         <v>500</v>
       </c>
@@ -21010,7 +21064,7 @@
         <v>208</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21022,7 +21076,7 @@
         <f>B24*0.0254</f>
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="D24" s="38"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="5">
         <v>1000</v>
       </c>
@@ -21042,7 +21096,7 @@
         <v>208</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21053,7 +21107,7 @@
       <c r="C25" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="5">
         <v>1800</v>
       </c>
@@ -21073,7 +21127,7 @@
         <v>208</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21085,7 +21139,7 @@
         <f>B26*4.44822</f>
         <v>4.4482200000000001</v>
       </c>
-      <c r="D26" s="38"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="5">
         <v>2000</v>
       </c>
@@ -21102,11 +21156,11 @@
         <v>2.5130890052356021</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" ref="J26:J31" si="16">F26*$J$22/$F$22</f>
+        <f t="shared" ref="J26:J31" si="20">F26*$J$22/$F$22</f>
         <v>187.2</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21117,7 +21171,7 @@
       <c r="C27" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="38"/>
+      <c r="D27" s="43"/>
       <c r="E27" s="5">
         <v>2500</v>
       </c>
@@ -21134,11 +21188,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>149.76</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21150,7 +21204,7 @@
         <f>B28/2.23694</f>
         <v>22.351962949386213</v>
       </c>
-      <c r="D28" s="38"/>
+      <c r="D28" s="43"/>
       <c r="E28" s="5">
         <v>3000</v>
       </c>
@@ -21167,11 +21221,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>124.8</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>59.428571428571445</v>
       </c>
     </row>
@@ -21182,7 +21236,7 @@
       <c r="C29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="38"/>
+      <c r="D29" s="43"/>
       <c r="E29" s="5">
         <v>3500</v>
       </c>
@@ -21199,11 +21253,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>106.97142857142858</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>50.938775510204088</v>
       </c>
     </row>
@@ -21215,7 +21269,7 @@
         <f>B30*0.277778</f>
         <v>27.777800000000003</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="43"/>
       <c r="E30" s="5">
         <v>4000</v>
       </c>
@@ -21232,11 +21286,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>93.6</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>44.571428571428577</v>
       </c>
     </row>
@@ -21247,7 +21301,7 @@
       <c r="C31" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="38"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="5">
         <v>4500</v>
       </c>
@@ -21264,11 +21318,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>83.2</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>39.619047619047628</v>
       </c>
     </row>
@@ -21280,7 +21334,7 @@
         <f>B32*1.35582</f>
         <v>1.35582</v>
       </c>
-      <c r="D32" s="38"/>
+      <c r="D32" s="43"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -21295,17 +21349,17 @@
       <c r="C33" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="38"/>
-      <c r="E33" s="52" t="s">
+      <c r="D33" s="43"/>
+      <c r="E33" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="31">
@@ -21315,7 +21369,7 @@
         <f>B34*0.7457</f>
         <v>0.74570000000000003</v>
       </c>
-      <c r="D34" s="38"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="4" t="s">
         <v>50</v>
       </c>
@@ -21343,7 +21397,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="33"/>
-      <c r="D35" s="38"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="5">
         <v>0</v>
       </c>
@@ -21363,7 +21417,7 @@
         <v>384</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" ref="K35:K44" si="17">H35*$J$35/$F$35</f>
+        <f t="shared" ref="K35:K44" si="21">H35*$J$35/$F$35</f>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21374,7 +21428,7 @@
       <c r="C36" s="28">
         <v>100</v>
       </c>
-      <c r="D36" s="38"/>
+      <c r="D36" s="43"/>
       <c r="E36" s="5">
         <v>500</v>
       </c>
@@ -21391,11 +21445,11 @@
         <v>0.94240837696335078</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" ref="J36:J44" si="18">F36*$J$35/$F$35</f>
+        <f t="shared" ref="J36:J44" si="22">F36*$J$35/$F$35</f>
         <v>384</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21406,7 +21460,7 @@
       <c r="C37" s="28">
         <v>16</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="43"/>
       <c r="E37" s="5">
         <v>1000</v>
       </c>
@@ -21423,11 +21477,11 @@
         <v>1.8848167539267016</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>384</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21439,7 +21493,7 @@
         <f>1000*C36/3600/C37</f>
         <v>1.7361111111111112</v>
       </c>
-      <c r="D38" s="38"/>
+      <c r="D38" s="43"/>
       <c r="E38" s="5">
         <v>1500</v>
       </c>
@@ -21456,16 +21510,16 @@
         <v>2.8272251308900525</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>384</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="38"/>
+      <c r="D39" s="43"/>
       <c r="E39" s="5">
         <v>2000</v>
       </c>
@@ -21482,11 +21536,11 @@
         <v>3.7696335078534031</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>384</v>
       </c>
       <c r="K39" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21500,7 +21554,7 @@
       <c r="C40" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="38"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="5">
         <v>2650</v>
       </c>
@@ -21517,16 +21571,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>289.81132075471697</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="38"/>
+      <c r="D41" s="43"/>
       <c r="E41" s="5">
         <v>3000</v>
       </c>
@@ -21543,16 +21597,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>256</v>
       </c>
       <c r="K41" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>105.26896551724138</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="38"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="5">
         <v>3500</v>
       </c>
@@ -21569,16 +21623,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>219.42857142857147</v>
       </c>
       <c r="K42" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>90.23054187192119</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="38"/>
+      <c r="D43" s="43"/>
       <c r="E43" s="5">
         <v>4000</v>
       </c>
@@ -21595,16 +21649,16 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>192</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>78.951724137931052</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D44" s="38"/>
+      <c r="D44" s="43"/>
       <c r="E44" s="5">
         <v>4500</v>
       </c>
@@ -21621,11 +21675,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>170.66666666666669</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>70.179310344827584</v>
       </c>
     </row>
@@ -21638,16 +21692,16 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E46" s="52" t="s">
+      <c r="E46" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
     </row>
     <row r="47" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
@@ -21693,7 +21747,7 @@
         <v>638</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" ref="K48:K60" si="19">H48*$J$48/$F$48</f>
+        <f t="shared" ref="K48:K60" si="23">H48*$J$48/$F$48</f>
         <v>239.25</v>
       </c>
     </row>
@@ -21714,11 +21768,11 @@
         <v>1.5706806282722514</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" ref="J49:J60" si="20">F49*$J$48/$F$48</f>
+        <f t="shared" ref="J49:J60" si="24">F49*$J$48/$F$48</f>
         <v>638</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21739,11 +21793,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>638</v>
       </c>
       <c r="K50" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21764,11 +21818,11 @@
         <v>4.7120418848167542</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>638</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21789,11 +21843,11 @@
         <v>6.2827225130890056</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>638</v>
       </c>
       <c r="K52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21814,11 +21868,11 @@
         <v>7.5392670157068062</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>638</v>
       </c>
       <c r="K53" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21839,11 +21893,11 @@
         <v>8.167539267015707</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>588.92307692307691</v>
       </c>
       <c r="K54" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21864,11 +21918,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>483.02839116719241</v>
       </c>
       <c r="K55" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21889,11 +21943,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>382.8</v>
       </c>
       <c r="K56" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>189.60562499999997</v>
       </c>
     </row>
@@ -21914,11 +21968,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>340.26666666666665</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>168.53833333333333</v>
       </c>
     </row>
@@ -21939,11 +21993,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>306.24</v>
       </c>
       <c r="K58" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>151.68450000000001</v>
       </c>
     </row>
@@ -21964,11 +22018,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>278.39999999999998</v>
       </c>
       <c r="K59" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>137.89499999999998</v>
       </c>
     </row>
@@ -21989,27 +22043,27 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>255.2</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>126.40374999999999</v>
       </c>
     </row>
     <row r="61" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="5:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E62" s="52" t="s">
+      <c r="E62" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="52"/>
-      <c r="M62" s="52"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="41"/>
+      <c r="K62" s="41"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41"/>
     </row>
     <row r="63" spans="5:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E63" s="19" t="s">
@@ -22506,16 +22560,16 @@
     </row>
     <row r="80" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="5:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E81" s="52" t="s">
+      <c r="E81" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="F81" s="52"/>
-      <c r="G81" s="52"/>
-      <c r="H81" s="52"/>
-      <c r="I81" s="52"/>
-      <c r="J81" s="52"/>
-      <c r="K81" s="52"/>
-      <c r="L81" s="52"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="41"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="41"/>
+      <c r="K81" s="41"/>
+      <c r="L81" s="41"/>
     </row>
     <row r="82" spans="5:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E82" s="4" t="s">
@@ -23302,16 +23356,16 @@
     </row>
     <row r="110" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="5:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E111" s="52" t="s">
+      <c r="E111" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="F111" s="52"/>
-      <c r="G111" s="52"/>
-      <c r="H111" s="52"/>
-      <c r="I111" s="52"/>
-      <c r="J111" s="52"/>
-      <c r="K111" s="52"/>
-      <c r="L111" s="52"/>
+      <c r="F111" s="41"/>
+      <c r="G111" s="41"/>
+      <c r="H111" s="41"/>
+      <c r="I111" s="41"/>
+      <c r="J111" s="41"/>
+      <c r="K111" s="41"/>
+      <c r="L111" s="41"/>
     </row>
     <row r="112" spans="5:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E112" s="4" t="s">
@@ -23895,16 +23949,16 @@
     </row>
     <row r="132" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="5:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E133" s="52" t="s">
+      <c r="E133" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="F133" s="52"/>
-      <c r="G133" s="52"/>
-      <c r="H133" s="52"/>
-      <c r="I133" s="52"/>
-      <c r="J133" s="52"/>
-      <c r="K133" s="52"/>
-      <c r="L133" s="52"/>
+      <c r="F133" s="41"/>
+      <c r="G133" s="41"/>
+      <c r="H133" s="41"/>
+      <c r="I133" s="41"/>
+      <c r="J133" s="41"/>
+      <c r="K133" s="41"/>
+      <c r="L133" s="41"/>
     </row>
     <row r="134" spans="5:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E134" s="4" t="s">
@@ -24401,16 +24455,16 @@
     </row>
     <row r="152" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="153" spans="5:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E153" s="52" t="s">
+      <c r="E153" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="F153" s="52"/>
-      <c r="G153" s="52"/>
-      <c r="H153" s="52"/>
-      <c r="I153" s="52"/>
-      <c r="J153" s="52"/>
-      <c r="K153" s="52"/>
-      <c r="L153" s="52"/>
+      <c r="F153" s="41"/>
+      <c r="G153" s="41"/>
+      <c r="H153" s="41"/>
+      <c r="I153" s="41"/>
+      <c r="J153" s="41"/>
+      <c r="K153" s="41"/>
+      <c r="L153" s="41"/>
     </row>
     <row r="154" spans="5:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E154" s="4" t="s">
@@ -24578,7 +24632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AE949E-7169-46AC-B298-A5EDE4A34403}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
@@ -24594,7 +24648,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C28" sqref="C28:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24641,31 +24695,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="51">
         <v>15000</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="51">
         <v>300</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="51">
         <v>1330</v>
       </c>
       <c r="E2" s="12">
         <v>1.35</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="51">
         <v>4000</v>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="51">
         <v>125</v>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="51">
         <v>250</v>
       </c>
       <c r="K2" s="15">
@@ -24673,26 +24727,26 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
       <c r="K3" s="16">
         <v>47.74</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="13">
         <v>3.5</v>
       </c>
@@ -24713,10 +24767,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="13">
         <v>4</v>
       </c>
@@ -24737,23 +24791,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="14">
         <v>4.43</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="51">
         <v>1106</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="51">
         <v>500</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="51">
         <v>1000</v>
       </c>
       <c r="K6" s="15">
@@ -24764,76 +24818,76 @@
       <c r="A7" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="48">
         <v>15000</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="48">
         <v>300</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="48">
         <v>4000</v>
       </c>
       <c r="E7" s="12">
         <v>5.2</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="18">
         <v>30.68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="13">
         <v>6.04</v>
       </c>
-      <c r="G8" s="40"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="18">
         <v>45.13</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="13">
         <v>7.04</v>
       </c>
-      <c r="G9" s="41"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
       <c r="K9" s="16">
         <v>50.62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="13">
         <v>8.08</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="51">
         <v>5000</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="51">
         <v>3500</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="51">
         <v>7000</v>
       </c>
       <c r="K10" s="15">
@@ -24841,81 +24895,81 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="13">
         <v>9.1</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
       <c r="K11" s="18">
         <v>24.92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="13">
         <v>10.11</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
       <c r="K12" s="18">
         <v>25.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="13">
         <v>11.05</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
       <c r="K13" s="18">
         <v>47.6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="13">
         <v>11.9</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
       <c r="K14" s="18">
         <v>57.49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="14">
         <v>13.35</v>
       </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
       <c r="K15" s="16">
         <v>64.08</v>
       </c>
@@ -24924,13 +24978,13 @@
       <c r="A16" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="48">
         <v>12000</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="48">
         <v>600</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="48">
         <v>2100</v>
       </c>
       <c r="E16" s="12">
@@ -24938,28 +24992,28 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="13">
         <v>1.97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="13">
         <v>2.88</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="14">
         <v>3.5</v>
       </c>
@@ -24968,13 +25022,13 @@
       <c r="A20" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="48">
         <v>12000</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="48">
         <v>600</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="48">
         <v>6500</v>
       </c>
       <c r="E20" s="12">
@@ -24982,64 +25036,64 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="13">
         <v>7.42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="13">
         <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="13">
         <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="13">
         <v>9.94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="13">
         <v>10.79</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="13">
         <v>12.36</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="14">
         <v>13.32</v>
       </c>
@@ -25048,13 +25102,13 @@
       <c r="A28" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28" s="48">
         <v>7500</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="48">
         <v>1200</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="48">
         <v>4770</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -25062,37 +25116,37 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="13">
         <v>2.97</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="14">
         <v>3.94</v>
       </c>
@@ -25101,29 +25155,29 @@
       <c r="A33" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47">
+      <c r="B33" s="48"/>
+      <c r="C33" s="48">
         <v>265</v>
       </c>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="12">
         <v>2.98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="13">
         <v>3.98</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="14">
         <v>6.03</v>
       </c>
@@ -25132,13 +25186,13 @@
       <c r="A36" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="47">
+      <c r="B36" s="48">
         <v>12500</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="48" t="s">
         <v>74</v>
       </c>
       <c r="E36" s="12">
@@ -25146,10 +25200,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="14">
         <v>6</v>
       </c>
@@ -25158,13 +25212,13 @@
       <c r="A38" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="47">
+      <c r="B38" s="48">
         <v>12500</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="D38" s="48" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="12">
@@ -25172,33 +25226,27 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="14">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="D7:D15"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -25215,17 +25263,23 @@
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B27"/>
     <mergeCell ref="C20:C27"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -25242,6 +25296,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63d68cde8d91d9cfd93ef1e7c2dce69f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490d39c642ce3fbaaaf8418555bb1ddb" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -25458,12 +25518,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
   <ds:schemaRefs>
@@ -25473,6 +25527,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08470758-3E41-49AE-BF09-F8ECFDDA61D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25489,13 +25552,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
started adding motor and battery sizing
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ElectricMotors\Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838DF4F0-C78B-4A37-A7D7-AD785BCAB201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BD40EA-3990-4040-8A71-531EEF31C58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -810,22 +810,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -837,13 +828,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -18914,16 +18914,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>61911</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>300036</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18950,16 +18950,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19525,10 +19525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335F5D5-EBE0-44CD-9439-894D8E00CE51}">
-  <dimension ref="A1:Z164"/>
+  <dimension ref="A1:AB164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19542,7 +19542,7 @@
     <col min="23" max="23" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
@@ -19622,7 +19622,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
@@ -19708,11 +19708,17 @@
         <f>W2*$B$16</f>
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="40">
         <v>600</v>
       </c>
+      <c r="Z2" s="40">
+        <f>1000*X2/Y2</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
@@ -19801,11 +19807,17 @@
         <f t="shared" ref="X3:X15" si="16">W3*$B$16</f>
         <v>21.83435957894736</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="40">
         <v>600</v>
       </c>
+      <c r="Z3" s="40">
+        <f t="shared" ref="Z3:Z15" si="17">1000*X3/Y3</f>
+        <v>36.390599298245604</v>
+      </c>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>13</v>
       </c>
@@ -19817,7 +19829,7 @@
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="20">
-        <f t="shared" ref="E4:E15" si="17">E3+$B$40</f>
+        <f t="shared" ref="E4:E15" si="18">E3+$B$40</f>
         <v>20</v>
       </c>
       <c r="F4" s="20">
@@ -19894,11 +19906,17 @@
         <f t="shared" si="16"/>
         <v>44.433950315789474</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="40">
         <v>600</v>
       </c>
+      <c r="Z4" s="40">
+        <f t="shared" si="17"/>
+        <v>74.056583859649123</v>
+      </c>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
@@ -19910,7 +19928,7 @@
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="F5" s="20">
@@ -19987,11 +20005,17 @@
         <f t="shared" si="16"/>
         <v>68.564003368421055</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="40">
         <v>600</v>
       </c>
+      <c r="Z5" s="40">
+        <f t="shared" si="17"/>
+        <v>114.27333894736842</v>
+      </c>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>15</v>
       </c>
@@ -20001,7 +20025,7 @@
       <c r="C6" s="26"/>
       <c r="D6" s="43"/>
       <c r="E6" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="F6" s="20">
@@ -20078,11 +20102,17 @@
         <f t="shared" si="16"/>
         <v>94.98974989473686</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="40">
         <v>600</v>
       </c>
+      <c r="Z6" s="40">
+        <f t="shared" si="17"/>
+        <v>158.31624982456142</v>
+      </c>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="40"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>123</v>
       </c>
@@ -20092,7 +20122,7 @@
       <c r="C7" s="26"/>
       <c r="D7" s="43"/>
       <c r="E7" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>50</v>
       </c>
       <c r="F7" s="20">
@@ -20169,11 +20199,17 @@
         <f t="shared" si="16"/>
         <v>124.47642105263157</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="40">
         <v>600</v>
       </c>
+      <c r="Z7" s="40">
+        <f t="shared" si="17"/>
+        <v>207.46070175438592</v>
+      </c>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="40"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
@@ -20183,7 +20219,7 @@
       <c r="C8" s="26"/>
       <c r="D8" s="43"/>
       <c r="E8" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>60</v>
       </c>
       <c r="F8" s="20">
@@ -20260,11 +20296,17 @@
         <f t="shared" si="16"/>
         <v>96.0065884433684</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="40">
         <v>600</v>
       </c>
+      <c r="Z8" s="40">
+        <f t="shared" si="17"/>
+        <v>160.01098073894732</v>
+      </c>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="40"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
@@ -20276,7 +20318,7 @@
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>70</v>
       </c>
       <c r="F9" s="20">
@@ -20353,11 +20395,17 @@
         <f t="shared" si="16"/>
         <v>39.455009495999995</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="40">
         <v>600</v>
       </c>
+      <c r="Z9" s="40">
+        <f t="shared" si="17"/>
+        <v>65.758349159999995</v>
+      </c>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>12</v>
       </c>
@@ -20367,7 +20415,7 @@
       <c r="C10" s="26"/>
       <c r="D10" s="43"/>
       <c r="E10" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>80</v>
       </c>
       <c r="F10" s="20">
@@ -20444,11 +20492,17 @@
         <f t="shared" si="16"/>
         <v>39.455009495999995</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="40">
         <v>600</v>
       </c>
+      <c r="Z10" s="40">
+        <f t="shared" si="17"/>
+        <v>65.758349159999995</v>
+      </c>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="40"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>128</v>
       </c>
@@ -20460,7 +20514,7 @@
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>90</v>
       </c>
       <c r="F11" s="24">
@@ -20537,11 +20591,17 @@
         <f t="shared" si="16"/>
         <v>2.3056414073317096E-2</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="38">
         <v>600</v>
       </c>
+      <c r="Z11" s="38">
+        <f t="shared" si="17"/>
+        <v>3.8427356788861826E-2</v>
+      </c>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>129</v>
       </c>
@@ -20553,7 +20613,7 @@
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="F12" s="22">
@@ -20578,7 +20638,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="22">
-        <f t="shared" ref="L12:L15" si="18">ATAN2(100, K12)</f>
+        <f t="shared" ref="L12:L15" si="19">ATAN2(100, K12)</f>
         <v>4.9958395721942765E-2</v>
       </c>
       <c r="M12" s="22">
@@ -20629,11 +20689,17 @@
         <f t="shared" si="16"/>
         <v>12.948986102386463</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="39">
         <v>600</v>
       </c>
+      <c r="Z12" s="39">
+        <f t="shared" si="17"/>
+        <v>21.581643503977439</v>
+      </c>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>130</v>
       </c>
@@ -20645,7 +20711,7 @@
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>110</v>
       </c>
       <c r="F13" s="22">
@@ -20670,7 +20736,7 @@
         <v>10</v>
       </c>
       <c r="L13" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9.9668652491162038E-2</v>
       </c>
       <c r="M13" s="22">
@@ -20721,11 +20787,17 @@
         <f t="shared" si="16"/>
         <v>12.095748117815699</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="39">
         <v>600</v>
       </c>
+      <c r="Z13" s="39">
+        <f t="shared" si="17"/>
+        <v>20.159580196359499</v>
+      </c>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>17</v>
       </c>
@@ -20737,7 +20809,7 @@
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>120</v>
       </c>
       <c r="F14" s="22">
@@ -20762,7 +20834,7 @@
         <v>20</v>
       </c>
       <c r="L14" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.19739555984988078</v>
       </c>
       <c r="M14" s="22">
@@ -20813,11 +20885,17 @@
         <f t="shared" si="16"/>
         <v>18.446151565269972</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="39">
         <v>600</v>
       </c>
+      <c r="Z14" s="39">
+        <f t="shared" si="17"/>
+        <v>30.743585942116617</v>
+      </c>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>18</v>
       </c>
@@ -20829,7 +20907,7 @@
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>130</v>
       </c>
       <c r="F15" s="22">
@@ -20856,7 +20934,7 @@
         <v>20</v>
       </c>
       <c r="L15" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.19739555984988078</v>
       </c>
       <c r="M15" s="22">
@@ -20907,11 +20985,17 @@
         <f t="shared" si="16"/>
         <v>6.9169780267130818</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="39">
         <v>600</v>
       </c>
+      <c r="Z15" s="39">
+        <f t="shared" si="17"/>
+        <v>11.528296711188469</v>
+      </c>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="39"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>32</v>
       </c>
@@ -21033,7 +21117,7 @@
         <v>208</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" ref="K22:K31" si="19">H22*$J$22/$F$22</f>
+        <f t="shared" ref="K22:K31" si="20">H22*$J$22/$F$22</f>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21064,7 +21148,7 @@
         <v>208</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21096,7 +21180,7 @@
         <v>208</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21127,7 +21211,7 @@
         <v>208</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21156,11 +21240,11 @@
         <v>2.5130890052356021</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" ref="J26:J31" si="20">F26*$J$22/$F$22</f>
+        <f t="shared" ref="J26:J31" si="21">F26*$J$22/$F$22</f>
         <v>187.2</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21188,11 +21272,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J27" s="1">
+        <f t="shared" si="21"/>
+        <v>149.76</v>
+      </c>
+      <c r="K27" s="1">
         <f t="shared" si="20"/>
-        <v>149.76</v>
-      </c>
-      <c r="K27" s="1">
-        <f t="shared" si="19"/>
         <v>71.314285714285717</v>
       </c>
     </row>
@@ -21221,11 +21305,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J28" s="1">
+        <f t="shared" si="21"/>
+        <v>124.8</v>
+      </c>
+      <c r="K28" s="1">
         <f t="shared" si="20"/>
-        <v>124.8</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" si="19"/>
         <v>59.428571428571445</v>
       </c>
     </row>
@@ -21253,11 +21337,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J29" s="1">
+        <f t="shared" si="21"/>
+        <v>106.97142857142858</v>
+      </c>
+      <c r="K29" s="1">
         <f t="shared" si="20"/>
-        <v>106.97142857142858</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" si="19"/>
         <v>50.938775510204088</v>
       </c>
     </row>
@@ -21286,11 +21370,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J30" s="1">
+        <f t="shared" si="21"/>
+        <v>93.6</v>
+      </c>
+      <c r="K30" s="1">
         <f t="shared" si="20"/>
-        <v>93.6</v>
-      </c>
-      <c r="K30" s="1">
-        <f t="shared" si="19"/>
         <v>44.571428571428577</v>
       </c>
     </row>
@@ -21318,11 +21402,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J31" s="1">
+        <f t="shared" si="21"/>
+        <v>83.2</v>
+      </c>
+      <c r="K31" s="1">
         <f t="shared" si="20"/>
-        <v>83.2</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="19"/>
         <v>39.619047619047628</v>
       </c>
     </row>
@@ -21417,7 +21501,7 @@
         <v>384</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" ref="K35:K44" si="21">H35*$J$35/$F$35</f>
+        <f t="shared" ref="K35:K44" si="22">H35*$J$35/$F$35</f>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21445,11 +21529,11 @@
         <v>0.94240837696335078</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" ref="J36:J44" si="22">F36*$J$35/$F$35</f>
+        <f t="shared" ref="J36:J44" si="23">F36*$J$35/$F$35</f>
         <v>384</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21477,11 +21561,11 @@
         <v>1.8848167539267016</v>
       </c>
       <c r="J37" s="1">
+        <f t="shared" si="23"/>
+        <v>384</v>
+      </c>
+      <c r="K37" s="1">
         <f t="shared" si="22"/>
-        <v>384</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21510,11 +21594,11 @@
         <v>2.8272251308900525</v>
       </c>
       <c r="J38" s="1">
+        <f t="shared" si="23"/>
+        <v>384</v>
+      </c>
+      <c r="K38" s="1">
         <f t="shared" si="22"/>
-        <v>384</v>
-      </c>
-      <c r="K38" s="1">
-        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21536,11 +21620,11 @@
         <v>3.7696335078534031</v>
       </c>
       <c r="J39" s="1">
+        <f t="shared" si="23"/>
+        <v>384</v>
+      </c>
+      <c r="K39" s="1">
         <f t="shared" si="22"/>
-        <v>384</v>
-      </c>
-      <c r="K39" s="1">
-        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21571,11 +21655,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J40" s="1">
+        <f t="shared" si="23"/>
+        <v>289.81132075471697</v>
+      </c>
+      <c r="K40" s="1">
         <f t="shared" si="22"/>
-        <v>289.81132075471697</v>
-      </c>
-      <c r="K40" s="1">
-        <f t="shared" si="21"/>
         <v>119.17241379310344</v>
       </c>
     </row>
@@ -21597,11 +21681,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J41" s="1">
+        <f t="shared" si="23"/>
+        <v>256</v>
+      </c>
+      <c r="K41" s="1">
         <f t="shared" si="22"/>
-        <v>256</v>
-      </c>
-      <c r="K41" s="1">
-        <f t="shared" si="21"/>
         <v>105.26896551724138</v>
       </c>
     </row>
@@ -21623,11 +21707,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J42" s="1">
+        <f t="shared" si="23"/>
+        <v>219.42857142857147</v>
+      </c>
+      <c r="K42" s="1">
         <f t="shared" si="22"/>
-        <v>219.42857142857147</v>
-      </c>
-      <c r="K42" s="1">
-        <f t="shared" si="21"/>
         <v>90.23054187192119</v>
       </c>
     </row>
@@ -21649,11 +21733,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J43" s="1">
+        <f t="shared" si="23"/>
+        <v>192</v>
+      </c>
+      <c r="K43" s="1">
         <f t="shared" si="22"/>
-        <v>192</v>
-      </c>
-      <c r="K43" s="1">
-        <f t="shared" si="21"/>
         <v>78.951724137931052</v>
       </c>
     </row>
@@ -21675,11 +21759,11 @@
         <v>4.994764397905759</v>
       </c>
       <c r="J44" s="1">
+        <f t="shared" si="23"/>
+        <v>170.66666666666669</v>
+      </c>
+      <c r="K44" s="1">
         <f t="shared" si="22"/>
-        <v>170.66666666666669</v>
-      </c>
-      <c r="K44" s="1">
-        <f t="shared" si="21"/>
         <v>70.179310344827584</v>
       </c>
     </row>
@@ -21747,7 +21831,7 @@
         <v>638</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" ref="K48:K60" si="23">H48*$J$48/$F$48</f>
+        <f t="shared" ref="K48:K60" si="24">H48*$J$48/$F$48</f>
         <v>239.25</v>
       </c>
     </row>
@@ -21768,11 +21852,11 @@
         <v>1.5706806282722514</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" ref="J49:J60" si="24">F49*$J$48/$F$48</f>
+        <f t="shared" ref="J49:J60" si="25">F49*$J$48/$F$48</f>
         <v>638</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21793,11 +21877,11 @@
         <v>3.1413612565445028</v>
       </c>
       <c r="J50" s="1">
+        <f t="shared" si="25"/>
+        <v>638</v>
+      </c>
+      <c r="K50" s="1">
         <f t="shared" si="24"/>
-        <v>638</v>
-      </c>
-      <c r="K50" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21818,11 +21902,11 @@
         <v>4.7120418848167542</v>
       </c>
       <c r="J51" s="1">
+        <f t="shared" si="25"/>
+        <v>638</v>
+      </c>
+      <c r="K51" s="1">
         <f t="shared" si="24"/>
-        <v>638</v>
-      </c>
-      <c r="K51" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21843,11 +21927,11 @@
         <v>6.2827225130890056</v>
       </c>
       <c r="J52" s="1">
+        <f t="shared" si="25"/>
+        <v>638</v>
+      </c>
+      <c r="K52" s="1">
         <f t="shared" si="24"/>
-        <v>638</v>
-      </c>
-      <c r="K52" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21868,11 +21952,11 @@
         <v>7.5392670157068062</v>
       </c>
       <c r="J53" s="1">
+        <f t="shared" si="25"/>
+        <v>638</v>
+      </c>
+      <c r="K53" s="1">
         <f t="shared" si="24"/>
-        <v>638</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21893,11 +21977,11 @@
         <v>8.167539267015707</v>
       </c>
       <c r="J54" s="1">
+        <f t="shared" si="25"/>
+        <v>588.92307692307691</v>
+      </c>
+      <c r="K54" s="1">
         <f t="shared" si="24"/>
-        <v>588.92307692307691</v>
-      </c>
-      <c r="K54" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21918,11 +22002,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J55" s="1">
+        <f t="shared" si="25"/>
+        <v>483.02839116719241</v>
+      </c>
+      <c r="K55" s="1">
         <f t="shared" si="24"/>
-        <v>483.02839116719241</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="23"/>
         <v>239.25</v>
       </c>
     </row>
@@ -21943,11 +22027,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J56" s="1">
+        <f t="shared" si="25"/>
+        <v>382.8</v>
+      </c>
+      <c r="K56" s="1">
         <f t="shared" si="24"/>
-        <v>382.8</v>
-      </c>
-      <c r="K56" s="1">
-        <f t="shared" si="23"/>
         <v>189.60562499999997</v>
       </c>
     </row>
@@ -21968,11 +22052,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J57" s="1">
+        <f t="shared" si="25"/>
+        <v>340.26666666666665</v>
+      </c>
+      <c r="K57" s="1">
         <f t="shared" si="24"/>
-        <v>340.26666666666665</v>
-      </c>
-      <c r="K57" s="1">
-        <f t="shared" si="23"/>
         <v>168.53833333333333</v>
       </c>
     </row>
@@ -21993,11 +22077,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J58" s="1">
+        <f t="shared" si="25"/>
+        <v>306.24</v>
+      </c>
+      <c r="K58" s="1">
         <f t="shared" si="24"/>
-        <v>306.24</v>
-      </c>
-      <c r="K58" s="1">
-        <f t="shared" si="23"/>
         <v>151.68450000000001</v>
       </c>
     </row>
@@ -22018,11 +22102,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J59" s="1">
+        <f t="shared" si="25"/>
+        <v>278.39999999999998</v>
+      </c>
+      <c r="K59" s="1">
         <f t="shared" si="24"/>
-        <v>278.39999999999998</v>
-      </c>
-      <c r="K59" s="1">
-        <f t="shared" si="23"/>
         <v>137.89499999999998</v>
       </c>
     </row>
@@ -22043,11 +22127,11 @@
         <v>9.9581151832460737</v>
       </c>
       <c r="J60" s="1">
+        <f t="shared" si="25"/>
+        <v>255.2</v>
+      </c>
+      <c r="K60" s="1">
         <f t="shared" si="24"/>
-        <v>255.2</v>
-      </c>
-      <c r="K60" s="1">
-        <f t="shared" si="23"/>
         <v>126.40374999999999</v>
       </c>
     </row>
@@ -24632,7 +24716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AE949E-7169-46AC-B298-A5EDE4A34403}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
@@ -24695,31 +24779,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="48">
         <v>15000</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="48">
         <v>300</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="48">
         <v>1330</v>
       </c>
       <c r="E2" s="12">
         <v>1.35</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="51">
+      <c r="H2" s="48">
         <v>4000</v>
       </c>
-      <c r="I2" s="51">
+      <c r="I2" s="48">
         <v>125</v>
       </c>
-      <c r="J2" s="51">
+      <c r="J2" s="48">
         <v>250</v>
       </c>
       <c r="K2" s="15">
@@ -24727,26 +24811,26 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="16">
         <v>47.74</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="13">
         <v>3.5</v>
       </c>
@@ -24767,10 +24851,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="13">
         <v>4</v>
       </c>
@@ -24791,23 +24875,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="14">
         <v>4.43</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="48">
         <v>1106</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="48">
         <v>500</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="48">
         <v>1000</v>
       </c>
       <c r="K6" s="15">
@@ -24815,79 +24899,79 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="53">
         <v>15000</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="53">
         <v>300</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="53">
         <v>4000</v>
       </c>
       <c r="E7" s="12">
         <v>5.2</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="18">
         <v>30.68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="13">
         <v>6.04</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="18">
         <v>45.13</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
       <c r="E9" s="13">
         <v>7.04</v>
       </c>
-      <c r="G9" s="56"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
       <c r="K9" s="16">
         <v>50.62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="13">
         <v>8.08</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="48">
         <v>5000</v>
       </c>
-      <c r="I10" s="51">
+      <c r="I10" s="48">
         <v>3500</v>
       </c>
-      <c r="J10" s="51">
+      <c r="J10" s="48">
         <v>7000</v>
       </c>
       <c r="K10" s="15">
@@ -24895,96 +24979,96 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="13">
         <v>9.1</v>
       </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
       <c r="K11" s="18">
         <v>24.92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="13">
         <v>10.11</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
       <c r="K12" s="18">
         <v>25.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="13">
         <v>11.05</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
       <c r="K13" s="18">
         <v>47.6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="13">
         <v>11.9</v>
       </c>
-      <c r="G14" s="55"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
       <c r="K14" s="18">
         <v>57.49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="14">
         <v>13.35</v>
       </c>
-      <c r="G15" s="56"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="16">
         <v>64.08</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="53">
         <v>12000</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="53">
         <v>600</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="53">
         <v>2100</v>
       </c>
       <c r="E16" s="12">
@@ -24992,43 +25076,43 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="13">
         <v>1.97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="13">
         <v>2.88</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="14">
         <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B20" s="53">
         <v>12000</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="53">
         <v>600</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="53">
         <v>6500</v>
       </c>
       <c r="E20" s="12">
@@ -25036,79 +25120,79 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
       <c r="E21" s="13">
         <v>7.42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
       <c r="E22" s="13">
         <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="13">
         <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="13">
         <v>9.94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="13">
         <v>10.79</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="13">
         <v>12.36</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="14">
         <v>13.32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="53">
         <v>7500</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="53">
         <v>1200</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="53">
         <v>4770</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -25116,83 +25200,83 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
       <c r="E29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="13">
         <v>2.97</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="14">
         <v>3.94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48">
+      <c r="B33" s="53"/>
+      <c r="C33" s="53">
         <v>265</v>
       </c>
-      <c r="D33" s="48"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="12">
         <v>2.98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
       <c r="E34" s="13">
         <v>3.98</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="47"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="14">
         <v>6.03</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="48">
+      <c r="B36" s="53">
         <v>12500</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="53" t="s">
         <v>74</v>
       </c>
       <c r="E36" s="12">
@@ -25200,25 +25284,25 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="48">
+      <c r="B38" s="53">
         <v>12500</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="53" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="12">
@@ -25226,27 +25310,33 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
       <c r="E39" s="14">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -25263,23 +25353,17 @@
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B27"/>
     <mergeCell ref="C20:C27"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -25296,12 +25380,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63d68cde8d91d9cfd93ef1e7c2dce69f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490d39c642ce3fbaaaf8418555bb1ddb" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -25518,6 +25596,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
   <ds:schemaRefs>
@@ -25527,15 +25611,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08470758-3E41-49AE-BF09-F8ECFDDA61D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25552,4 +25627,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
need to fix the data in the figure
</commit_message>
<xml_diff>
--- a/Sizing/Sizing.xlsx
+++ b/Sizing/Sizing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Omni\ElectricMotors\Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700D1F9A-F7A8-46F7-AE9F-0C7D6C4FE5F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1AE924-2854-4167-9FAE-BD1C889C81D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0626AE80-454B-4539-8E37-8436CB968B23}"/>
   </bookViews>
@@ -877,13 +877,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -895,22 +904,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyAlignment="1">
@@ -1396,7 +1396,7 @@
                   <c:v>2.2498493684210525</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.35393218724873071</c:v>
+                  <c:v>0.48749857020601195</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0.55273983098729895</c:v>
@@ -2216,70 +2216,70 @@
                   <c:v>99.776617712426912</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>99.773001349155152</c:v>
+                  <c:v>99.772815840289908</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>99.771742082463135</c:v>
+                  <c:v>99.771371064732705</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>99.76982281372571</c:v>
+                  <c:v>99.769451795995295</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>99.7671357444965</c:v>
+                  <c:v>99.766764726766056</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>99.763680781778618</c:v>
+                  <c:v>99.763309764048174</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>99.759457806004704</c:v>
+                  <c:v>99.759086788274274</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>99.754466671036894</c:v>
+                  <c:v>99.754095653306464</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>99.748707204166735</c:v>
+                  <c:v>99.748336186436305</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>99.742179206115296</c:v>
+                  <c:v>99.741808188384866</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>99.734882451033116</c:v>
+                  <c:v>99.734511433302657</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>99.726816686500158</c:v>
+                  <c:v>99.726445668769728</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>99.717981633525909</c:v>
+                  <c:v>99.717610615795508</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>99.708376986549339</c:v>
+                  <c:v>99.70800596881891</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>99.698002413438886</c:v>
+                  <c:v>99.697631395708427</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>99.686857555492367</c:v>
+                  <c:v>99.686486537761922</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>99.674942027437211</c:v>
+                  <c:v>99.674571009706767</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>99.662255417430231</c:v>
+                  <c:v>99.661884399699801</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>99.648797287057775</c:v>
+                  <c:v>99.648426269327345</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>99.634567171335604</c:v>
+                  <c:v>99.634196153605174</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>99.619564578709003</c:v>
+                  <c:v>99.619193560978559</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>99.603788991052696</c:v>
+                  <c:v>99.603417973322266</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>99.587626773028902</c:v>
+                  <c:v>99.587255755298457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2653,70 +2653,70 @@
                   <c:v>0.22338228757309952</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.22699865084486306</c:v>
+                  <c:v>0.22718415971008152</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.22825791753685756</c:v>
+                  <c:v>0.22862893526729444</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.23017718627427691</c:v>
+                  <c:v>0.23054820400471382</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.23286425550350612</c:v>
+                  <c:v>0.23323527323394302</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.23631921822138729</c:v>
+                  <c:v>0.23669023595182417</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.24054219399528881</c:v>
+                  <c:v>0.24091321172572569</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.24553332896310545</c:v>
+                  <c:v>0.2459043466935423</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.25129279583325825</c:v>
+                  <c:v>0.2516638135636951</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.25782079388469459</c:v>
+                  <c:v>0.25819181161513144</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.26511754896688811</c:v>
+                  <c:v>0.26548856669732496</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.27318331349983882</c:v>
+                  <c:v>0.27355433123027573</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.28201836647407308</c:v>
+                  <c:v>0.28238938420450999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.29162301345064351</c:v>
+                  <c:v>0.29199403118108042</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.30199758656112902</c:v>
+                  <c:v>0.30236860429156592</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.31314244450763495</c:v>
+                  <c:v>0.31351346223807186</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.32505797256279284</c:v>
+                  <c:v>0.32542899029322969</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.33774458256976053</c:v>
+                  <c:v>0.33811560030019738</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.35120271294222233</c:v>
+                  <c:v>0.35157373067265923</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.36543282866438864</c:v>
+                  <c:v>0.36580384639482555</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.38043542129099639</c:v>
+                  <c:v>0.3808064390214333</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.39621100894730882</c:v>
+                  <c:v>0.39658202667774567</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.41237322697110501</c:v>
+                  <c:v>0.41274424470154197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15243,7 +15243,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>30</c:v>
@@ -22078,9 +22078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335F5D5-EBE0-44CD-9439-894D8E00CE51}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22203,7 +22203,7 @@
         <v>125</v>
       </c>
       <c r="B11" s="20">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>15</v>
@@ -22541,7 +22541,7 @@
   <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
@@ -26234,7 +26234,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="36">
-        <f t="shared" ref="M34:M65" si="11">SUM(I34,J34,K34,L34)</f>
+        <f t="shared" ref="M34:M55" si="11">SUM(I34,J34,K34,L34)</f>
         <v>213.73569000000001</v>
       </c>
       <c r="N34" s="36">
@@ -26258,7 +26258,7 @@
         <v>3664.2649688599158</v>
       </c>
       <c r="S34" s="38">
-        <f t="shared" ref="S34:S65" si="13">Q34*R34*2*PI()/60/1000</f>
+        <f t="shared" ref="S34:S55" si="13">Q34*R34*2*PI()/60/1000</f>
         <v>2.2498493684210525</v>
       </c>
       <c r="T34" s="38">
@@ -26269,32 +26269,32 @@
         <v>600</v>
       </c>
       <c r="V34" s="38">
-        <f t="shared" ref="V34:V65" si="14">1000*T34/U34</f>
+        <f t="shared" ref="V34:V55" si="14">1000*T34/U34</f>
         <v>3.7497489473684209</v>
       </c>
       <c r="W34" s="38">
-        <f t="shared" ref="W34:W65" si="15">AVERAGE(V34:V35)</f>
-        <v>2.1698179630581529</v>
+        <f t="shared" ref="W34:W54" si="15">AVERAGE(V34:V35)</f>
+        <v>2.2811232821892204</v>
       </c>
       <c r="X34" s="38">
         <f>W34*Application!$B$44/3600</f>
-        <v>6.0272721196059798E-3</v>
+        <v>6.3364535616367238E-3</v>
       </c>
       <c r="Y34" s="38">
         <f>SUM($X$2:X34)</f>
-        <v>0.37833108474143845</v>
+        <v>0.37864026618346919</v>
       </c>
       <c r="Z34" s="36">
         <f>Application!$B$21*1000/Application!$B$20</f>
         <v>166.66666666666666</v>
       </c>
       <c r="AA34" s="36">
-        <f t="shared" ref="AA34:AA65" si="16">100*(Z34-Y34)/Z34</f>
-        <v>99.773001349155152</v>
+        <f t="shared" ref="AA34:AA55" si="16">100*(Z34-Y34)/Z34</f>
+        <v>99.772815840289908</v>
       </c>
       <c r="AB34" s="38">
         <f t="shared" ref="AB34:AB55" si="17">100*Y34/Z34</f>
-        <v>0.22699865084486306</v>
+        <v>0.22718415971008152</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.45">
@@ -26321,19 +26321,19 @@
       </c>
       <c r="G35" s="30">
         <f>Application!B11</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H35" s="30">
         <f t="shared" ref="H35:H55" si="19">ATAN2(100,G35)</f>
-        <v>0.3805063771123649</v>
+        <v>0.54041950027058416</v>
       </c>
       <c r="I35" s="30">
         <f>Application!$B$2*Application!$B$3*SIN(H35)</f>
-        <v>3304.511679275618</v>
+        <v>4577.81344819484</v>
       </c>
       <c r="J35" s="30">
         <f>Application!$B$2*Application!$B$3*Application!$B$7*COS(H35)</f>
-        <v>57.828954387323314</v>
+        <v>53.40782356227313</v>
       </c>
       <c r="K35" s="30">
         <f>0.5*Application!$B$5*Application!$B$6*Application!$B$4*D35^2</f>
@@ -26345,11 +26345,11 @@
       </c>
       <c r="M35" s="30">
         <f t="shared" si="11"/>
-        <v>3362.3557788629414</v>
+        <v>4631.2364169571129</v>
       </c>
       <c r="N35" s="30">
         <f>M35*Application!$B$9</f>
-        <v>1445.8129849110649</v>
+        <v>1991.4316592915584</v>
       </c>
       <c r="O35" s="30">
         <f>D35*60/2/PI()/Application!$B$9</f>
@@ -26361,7 +26361,7 @@
       </c>
       <c r="Q35" s="30">
         <f>N35/P35/Application!$B$17/Application!$B$10</f>
-        <v>92.236873040578303</v>
+        <v>127.04508193247582</v>
       </c>
       <c r="R35" s="30">
         <f t="shared" si="12"/>
@@ -26369,30 +26369,30 @@
       </c>
       <c r="S35" s="32">
         <f t="shared" si="13"/>
-        <v>0.35393218724873071</v>
+        <v>0.48749857020601195</v>
       </c>
       <c r="T35" s="32">
         <f>S35*Application!$B$17</f>
-        <v>0.35393218724873071</v>
+        <v>0.48749857020601195</v>
       </c>
       <c r="U35" s="32">
         <v>600</v>
       </c>
       <c r="V35" s="32">
         <f t="shared" si="14"/>
-        <v>0.58988697874788454</v>
+        <v>0.81249761701001988</v>
       </c>
       <c r="W35" s="32">
         <f t="shared" si="15"/>
-        <v>0.75556001519669147</v>
+        <v>0.86686533432775903</v>
       </c>
       <c r="X35" s="32">
         <f>W35*Application!$B$44/3600</f>
-        <v>2.0987778199908096E-3</v>
+        <v>2.4079592620215528E-3</v>
       </c>
       <c r="Y35" s="32">
         <f>SUM($X$2:X35)</f>
-        <v>0.38042986256142924</v>
+        <v>0.38104822544549072</v>
       </c>
       <c r="Z35" s="30">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26400,11 +26400,11 @@
       </c>
       <c r="AA35" s="30">
         <f t="shared" si="16"/>
-        <v>99.771742082463135</v>
+        <v>99.771371064732705</v>
       </c>
       <c r="AB35" s="32">
         <f t="shared" si="17"/>
-        <v>0.22825791753685756</v>
+        <v>0.22862893526729444</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.45">
@@ -26505,7 +26505,7 @@
       </c>
       <c r="Y36" s="35">
         <f>SUM($X$2:X36)</f>
-        <v>0.38362864379046152</v>
+        <v>0.384247006674523</v>
       </c>
       <c r="Z36" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26513,11 +26513,11 @@
       </c>
       <c r="AA36" s="33">
         <f t="shared" si="16"/>
-        <v>99.76982281372571</v>
+        <v>99.769451795995295</v>
       </c>
       <c r="AB36" s="35">
         <f t="shared" si="17"/>
-        <v>0.23017718627427691</v>
+        <v>0.23054820400471382</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.45">
@@ -26618,7 +26618,7 @@
       </c>
       <c r="Y37" s="35">
         <f>SUM($X$2:X37)</f>
-        <v>0.38810709250584352</v>
+        <v>0.38872545538990499</v>
       </c>
       <c r="Z37" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26626,11 +26626,11 @@
       </c>
       <c r="AA37" s="33">
         <f t="shared" si="16"/>
-        <v>99.7671357444965</v>
+        <v>99.766764726766056</v>
       </c>
       <c r="AB37" s="35">
         <f t="shared" si="17"/>
-        <v>0.23286425550350612</v>
+        <v>0.23323527323394302</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.45">
@@ -26731,7 +26731,7 @@
       </c>
       <c r="Y38" s="35">
         <f>SUM($X$2:X38)</f>
-        <v>0.39386536370231212</v>
+        <v>0.3944837265863736</v>
       </c>
       <c r="Z38" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26739,11 +26739,11 @@
       </c>
       <c r="AA38" s="33">
         <f t="shared" si="16"/>
-        <v>99.763680781778618</v>
+        <v>99.763309764048174</v>
       </c>
       <c r="AB38" s="35">
         <f t="shared" si="17"/>
-        <v>0.23631921822138729</v>
+        <v>0.23669023595182417</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.45">
@@ -26844,7 +26844,7 @@
       </c>
       <c r="Y39" s="35">
         <f>SUM($X$2:X39)</f>
-        <v>0.40090365665881467</v>
+        <v>0.40152201954287614</v>
       </c>
       <c r="Z39" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26852,11 +26852,11 @@
       </c>
       <c r="AA39" s="33">
         <f t="shared" si="16"/>
-        <v>99.759457806004704</v>
+        <v>99.759086788274274</v>
       </c>
       <c r="AB39" s="35">
         <f t="shared" si="17"/>
-        <v>0.24054219399528881</v>
+        <v>0.24091321172572569</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.45">
@@ -26957,7 +26957,7 @@
       </c>
       <c r="Y40" s="35">
         <f>SUM($X$2:X40)</f>
-        <v>0.40922221493850902</v>
+        <v>0.4098405778225705</v>
       </c>
       <c r="Z40" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -26965,11 +26965,11 @@
       </c>
       <c r="AA40" s="33">
         <f t="shared" si="16"/>
-        <v>99.754466671036894</v>
+        <v>99.754095653306464</v>
       </c>
       <c r="AB40" s="35">
         <f t="shared" si="17"/>
-        <v>0.24553332896310545</v>
+        <v>0.2459043466935423</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.45">
@@ -27070,7 +27070,7 @@
       </c>
       <c r="Y41" s="35">
         <f>SUM($X$2:X41)</f>
-        <v>0.41882132638876368</v>
+        <v>0.41943968927282516</v>
       </c>
       <c r="Z41" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27078,11 +27078,11 @@
       </c>
       <c r="AA41" s="33">
         <f t="shared" si="16"/>
-        <v>99.748707204166735</v>
+        <v>99.748336186436305</v>
       </c>
       <c r="AB41" s="35">
         <f t="shared" si="17"/>
-        <v>0.25129279583325825</v>
+        <v>0.2516638135636951</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.45">
@@ -27183,7 +27183,7 @@
       </c>
       <c r="Y42" s="35">
         <f>SUM($X$2:X42)</f>
-        <v>0.42970132314115755</v>
+        <v>0.43031968602521903</v>
       </c>
       <c r="Z42" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27191,11 +27191,11 @@
       </c>
       <c r="AA42" s="33">
         <f t="shared" si="16"/>
-        <v>99.742179206115296</v>
+        <v>99.741808188384866</v>
       </c>
       <c r="AB42" s="35">
         <f t="shared" si="17"/>
-        <v>0.25782079388469459</v>
+        <v>0.25819181161513144</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.45">
@@ -27296,7 +27296,7 @@
       </c>
       <c r="Y43" s="35">
         <f>SUM($X$2:X43)</f>
-        <v>0.44186258161148012</v>
+        <v>0.44248094449554159</v>
       </c>
       <c r="Z43" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27304,11 +27304,11 @@
       </c>
       <c r="AA43" s="33">
         <f t="shared" si="16"/>
-        <v>99.734882451033116</v>
+        <v>99.734511433302657</v>
       </c>
       <c r="AB43" s="35">
         <f t="shared" si="17"/>
-        <v>0.26511754896688811</v>
+        <v>0.26548856669732496</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.45">
@@ -27409,7 +27409,7 @@
       </c>
       <c r="Y44" s="35">
         <f>SUM($X$2:X44)</f>
-        <v>0.45530552249973133</v>
+        <v>0.4559238853837928</v>
       </c>
       <c r="Z44" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27417,11 +27417,11 @@
       </c>
       <c r="AA44" s="33">
         <f t="shared" si="16"/>
-        <v>99.726816686500158</v>
+        <v>99.726445668769728</v>
       </c>
       <c r="AB44" s="35">
         <f t="shared" si="17"/>
-        <v>0.27318331349983882</v>
+        <v>0.27355433123027573</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.45">
@@ -27522,7 +27522,7 @@
       </c>
       <c r="Y45" s="35">
         <f>SUM($X$2:X45)</f>
-        <v>0.47003061079012176</v>
+        <v>0.47064897367418324</v>
       </c>
       <c r="Z45" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27530,11 +27530,11 @@
       </c>
       <c r="AA45" s="33">
         <f t="shared" si="16"/>
-        <v>99.717981633525909</v>
+        <v>99.717610615795508</v>
       </c>
       <c r="AB45" s="35">
         <f t="shared" si="17"/>
-        <v>0.28201836647407308</v>
+        <v>0.28238938420450999</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.45">
@@ -27635,7 +27635,7 @@
       </c>
       <c r="Y46" s="35">
         <f>SUM($X$2:X46)</f>
-        <v>0.48603835575107246</v>
+        <v>0.48665671863513393</v>
       </c>
       <c r="Z46" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27643,11 +27643,11 @@
       </c>
       <c r="AA46" s="33">
         <f t="shared" si="16"/>
-        <v>99.708376986549339</v>
+        <v>99.70800596881891</v>
       </c>
       <c r="AB46" s="35">
         <f t="shared" si="17"/>
-        <v>0.29162301345064351</v>
+        <v>0.29199403118108042</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.45">
@@ -27748,7 +27748,7 @@
       </c>
       <c r="Y47" s="35">
         <f>SUM($X$2:X47)</f>
-        <v>0.50332931093521505</v>
+        <v>0.50394767381927652</v>
       </c>
       <c r="Z47" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27756,11 +27756,11 @@
       </c>
       <c r="AA47" s="33">
         <f t="shared" si="16"/>
-        <v>99.698002413438886</v>
+        <v>99.697631395708427</v>
       </c>
       <c r="AB47" s="35">
         <f t="shared" si="17"/>
-        <v>0.30199758656112902</v>
+        <v>0.30236860429156592</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.45">
@@ -27861,7 +27861,7 @@
       </c>
       <c r="Y48" s="35">
         <f>SUM($X$2:X48)</f>
-        <v>0.52190407417939155</v>
+        <v>0.52252243706345303</v>
       </c>
       <c r="Z48" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27869,11 +27869,11 @@
       </c>
       <c r="AA48" s="33">
         <f t="shared" si="16"/>
-        <v>99.686857555492367</v>
+        <v>99.686486537761922</v>
       </c>
       <c r="AB48" s="35">
         <f t="shared" si="17"/>
-        <v>0.31314244450763495</v>
+        <v>0.31351346223807186</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.45">
@@ -27974,7 +27974,7 @@
       </c>
       <c r="Y49" s="35">
         <f>SUM($X$2:X49)</f>
-        <v>0.54176328760465464</v>
+        <v>0.54238165048871612</v>
       </c>
       <c r="Z49" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -27982,11 +27982,11 @@
       </c>
       <c r="AA49" s="33">
         <f t="shared" si="16"/>
-        <v>99.674942027437211</v>
+        <v>99.674571009706767</v>
       </c>
       <c r="AB49" s="35">
         <f t="shared" si="17"/>
-        <v>0.32505797256279284</v>
+        <v>0.32542899029322969</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.45">
@@ -28087,7 +28087,7 @@
       </c>
       <c r="Y50" s="35">
         <f>SUM($X$2:X50)</f>
-        <v>0.5629076376162675</v>
+        <v>0.56352600050032897</v>
       </c>
       <c r="Z50" s="33">
         <f>Application!$B$21*1000/Application!$B$20</f>
@@ -28095,11 +28095,11 @@
       </c>
       <c r="AA50" s="33">
         <f t="shared" si="16"/>
-        <v>99.662255417430231</v>
+        <v>99.661884399699801</v>
       </c>
       <c r="AB50" s="35">
         <f t="shared" si="17"/>
-        <v>0.33774458256976053</v>
+        <v>0.33811560030019738</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.45">
@@ -28200,7 +28200,7 @@
       </c>
       <c r="Y51" s="35">
         <f>SUM($X$2:X51)</f>
-        <v>0.58533785490370382</v>
+        <v>0.5859562177877653</v>
       </c>
       <c r="Z51" s="33">
         <f>100*1000/600</f>
@@ -28208,11 +28208,11 @@
       </c>
       <c r="AA51" s="33">
         <f t="shared" si="16"/>
-        <v>99.648797287057775</v>
+        <v>99.648426269327345</v>
       </c>
       <c r="AB51" s="35">
         <f t="shared" si="17"/>
-        <v>0.35120271294222233</v>
+        <v>0.35157373067265923</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.45">
@@ -28313,7 +28313,7 @@
       </c>
       <c r="Y52" s="35">
         <f>SUM($X$2:X52)</f>
-        <v>0.60905471444064774</v>
+        <v>0.60967307732470921</v>
       </c>
       <c r="Z52" s="33">
         <f>100*1000/600</f>
@@ -28321,11 +28321,11 @@
       </c>
       <c r="AA52" s="33">
         <f t="shared" si="16"/>
-        <v>99.634567171335604</v>
+        <v>99.634196153605174</v>
       </c>
       <c r="AB52" s="35">
         <f t="shared" si="17"/>
-        <v>0.36543282866438864</v>
+        <v>0.36580384639482555</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.45">
@@ -28426,7 +28426,7 @@
       </c>
       <c r="Y53" s="35">
         <f>SUM($X$2:X53)</f>
-        <v>0.63405903548499398</v>
+        <v>0.63467739836905546</v>
       </c>
       <c r="Z53" s="33">
         <f>100*1000/600</f>
@@ -28434,11 +28434,11 @@
       </c>
       <c r="AA53" s="33">
         <f t="shared" si="16"/>
-        <v>99.619564578709003</v>
+        <v>99.619193560978559</v>
       </c>
       <c r="AB53" s="35">
         <f t="shared" si="17"/>
-        <v>0.38043542129099639</v>
+        <v>0.3808064390214333</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.45">
@@ -28539,7 +28539,7 @@
       </c>
       <c r="Y54" s="35">
         <f>SUM($X$2:X54)</f>
-        <v>0.66035168157884794</v>
+        <v>0.66097004446290941</v>
       </c>
       <c r="Z54" s="33">
         <f>100*1000/600</f>
@@ -28547,11 +28547,11 @@
       </c>
       <c r="AA54" s="33">
         <f t="shared" si="16"/>
-        <v>99.603788991052696</v>
+        <v>99.603417973322266</v>
       </c>
       <c r="AB54" s="35">
         <f t="shared" si="17"/>
-        <v>0.39621100894730882</v>
+        <v>0.39658202667774567</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.45">
@@ -28652,7 +28652,7 @@
       </c>
       <c r="Y55" s="35">
         <f>SUM($X$2:X55)</f>
-        <v>0.68728871161850835</v>
+        <v>0.68790707450256983</v>
       </c>
       <c r="Z55" s="33">
         <f>100*1000/600</f>
@@ -28660,11 +28660,11 @@
       </c>
       <c r="AA55" s="33">
         <f t="shared" si="16"/>
-        <v>99.587626773028902</v>
+        <v>99.587255755298457</v>
       </c>
       <c r="AB55" s="35">
         <f t="shared" si="17"/>
-        <v>0.41237322697110501</v>
+        <v>0.41274424470154197</v>
       </c>
     </row>
   </sheetData>
@@ -28739,31 +28739,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="47">
         <v>15000</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="47">
         <v>300</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="47">
         <v>1330</v>
       </c>
       <c r="E2" s="12">
         <v>1.35</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="47">
         <v>4000</v>
       </c>
-      <c r="I2" s="44">
+      <c r="I2" s="47">
         <v>125</v>
       </c>
-      <c r="J2" s="44">
+      <c r="J2" s="47">
         <v>250</v>
       </c>
       <c r="K2" s="15">
@@ -28771,26 +28771,26 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
       <c r="K3" s="16">
         <v>47.74</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="13">
         <v>3.5</v>
       </c>
@@ -28811,10 +28811,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="13">
         <v>4</v>
       </c>
@@ -28835,23 +28835,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14">
         <v>4.43</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="47">
         <v>1106</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="47">
         <v>500</v>
       </c>
-      <c r="J6" s="44">
+      <c r="J6" s="47">
         <v>1000</v>
       </c>
       <c r="K6" s="15">
@@ -28859,79 +28859,79 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="44">
         <v>15000</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="44">
         <v>300</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="44">
         <v>4000</v>
       </c>
       <c r="E7" s="12">
         <v>5.2</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="18">
         <v>30.68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="13">
         <v>6.04</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="18">
         <v>45.13</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="13">
         <v>7.04</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
       <c r="K9" s="16">
         <v>50.62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="13">
         <v>8.08</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="47">
         <v>5000</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="47">
         <v>3500</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="47">
         <v>7000</v>
       </c>
       <c r="K10" s="15">
@@ -28939,96 +28939,96 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="13">
         <v>9.1</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
       <c r="K11" s="18">
         <v>24.92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="13">
         <v>10.11</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="18">
         <v>25.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="13">
         <v>11.05</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="18">
         <v>47.6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="13">
         <v>11.9</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
       <c r="K14" s="18">
         <v>57.49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="14">
         <v>13.35</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
       <c r="K15" s="16">
         <v>64.08</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="44">
         <v>12000</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="44">
         <v>600</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="44">
         <v>2100</v>
       </c>
       <c r="E16" s="12">
@@ -29036,43 +29036,43 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="13">
         <v>1.97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="13">
         <v>2.88</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="48"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="14">
         <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="44">
         <v>12000</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="44">
         <v>600</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="44">
         <v>6500</v>
       </c>
       <c r="E20" s="12">
@@ -29080,79 +29080,79 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="13">
         <v>7.42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="13">
         <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="51"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="13">
         <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="13">
         <v>9.94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="51"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="13">
         <v>10.79</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="13">
         <v>12.36</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="48"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="14">
         <v>13.32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="49">
+      <c r="B28" s="44">
         <v>7500</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="44">
         <v>1200</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="44">
         <v>4770</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -29160,83 +29160,83 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
       <c r="E31" s="13">
         <v>2.97</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="48"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
       <c r="E32" s="14">
         <v>3.94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49">
+      <c r="B33" s="44"/>
+      <c r="C33" s="44">
         <v>265</v>
       </c>
-      <c r="D33" s="49"/>
+      <c r="D33" s="44"/>
       <c r="E33" s="12">
         <v>2.98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
       <c r="E34" s="13">
         <v>3.98</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="48"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
       <c r="E35" s="14">
         <v>6.03</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="49">
+      <c r="B36" s="44">
         <v>12500</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="44" t="s">
         <v>71</v>
       </c>
       <c r="E36" s="12">
@@ -29244,25 +29244,25 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="48"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="49">
+      <c r="B38" s="44">
         <v>12500</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="44" t="s">
         <v>71</v>
       </c>
       <c r="E38" s="12">
@@ -29270,33 +29270,27 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="48"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
       <c r="E39" s="14">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="D7:D15"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -29313,17 +29307,23 @@
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B27"/>
     <mergeCell ref="C20:C27"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -32852,6 +32852,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63d68cde8d91d9cfd93ef1e7c2dce69f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490d39c642ce3fbaaaf8418555bb1ddb" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -33068,12 +33074,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -33084,6 +33084,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08470758-3E41-49AE-BF09-F8ECFDDA61D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33102,15 +33111,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F324A3B8-30FC-4358-B87B-0224BB51D402}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31769C09-66BF-4C90-9A3A-4FD4D5E2DB91}">
   <ds:schemaRefs>

</xml_diff>